<commit_message>
Doc: updated the requirements status with ID CRS-SIQ_supplier_005 & 006 from pending to Yes
</commit_message>
<xml_diff>
--- a/Requirments/CRS-SIQ.xlsx
+++ b/Requirments/CRS-SIQ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI material\QA\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAD4DA7-8ACF-4860-8532-D348AC0161B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDFB163-0B62-4BD6-B1DC-2A2018B25796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -207,9 +207,6 @@
   <si>
     <t>As a supplier wants to add a new product all the product data is mandatory or there is some optional data
  (Ex:product id, product price &amp; product version are mandatory and product photo, product platform are Optional</t>
-  </si>
-  <si>
-    <t>Pending</t>
   </si>
   <si>
     <t>CRS-SIQ_supplier_006</t>
@@ -387,13 +384,13 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,20 +612,20 @@
   <dimension ref="A1:F1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="131.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="131.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="24.75" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,13 +635,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -654,11 +651,11 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -668,11 +665,11 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -682,11 +679,11 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -696,11 +693,11 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -710,11 +707,11 @@
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -724,11 +721,11 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -738,11 +735,11 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -752,11 +749,11 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -766,11 +763,11 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -780,11 +777,11 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -794,11 +791,11 @@
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -808,25 +805,25 @@
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -836,11 +833,11 @@
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
@@ -850,11 +847,11 @@
       <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -864,11 +861,11 @@
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
@@ -878,11 +875,11 @@
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -892,11 +889,11 @@
       <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
@@ -906,11 +903,11 @@
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
@@ -920,11 +917,11 @@
       <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
@@ -934,11 +931,11 @@
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
@@ -948,11 +945,11 @@
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>48</v>
       </c>
@@ -962,11 +959,11 @@
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>50</v>
       </c>
@@ -976,11 +973,11 @@
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>52</v>
       </c>
@@ -990,11 +987,11 @@
       <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>54</v>
       </c>
@@ -1004,11 +1001,11 @@
       <c r="C27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>56</v>
       </c>
@@ -1016,3001 +1013,3015 @@
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="C29" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="C31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C32" s="11"/>
     </row>
-    <row r="33" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C33" s="11"/>
     </row>
-    <row r="34" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C35" s="11"/>
     </row>
-    <row r="36" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C36" s="11"/>
     </row>
-    <row r="37" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C37" s="11"/>
     </row>
-    <row r="38" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C38" s="11"/>
     </row>
-    <row r="39" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C39" s="11"/>
     </row>
-    <row r="40" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C40" s="11"/>
     </row>
-    <row r="41" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C42" s="11"/>
     </row>
-    <row r="43" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C43" s="11"/>
     </row>
-    <row r="44" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C44" s="11"/>
     </row>
-    <row r="45" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="11"/>
     </row>
-    <row r="46" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="11"/>
     </row>
-    <row r="47" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="11"/>
     </row>
-    <row r="48" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="11"/>
     </row>
-    <row r="49" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="11"/>
     </row>
-    <row r="50" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="11"/>
     </row>
-    <row r="51" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="11"/>
     </row>
-    <row r="52" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="11"/>
     </row>
-    <row r="53" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="11"/>
     </row>
-    <row r="54" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="11"/>
     </row>
-    <row r="55" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="11"/>
     </row>
-    <row r="56" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="11"/>
     </row>
-    <row r="57" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="11"/>
     </row>
-    <row r="58" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="11"/>
     </row>
-    <row r="59" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="11"/>
     </row>
-    <row r="60" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="11"/>
     </row>
-    <row r="61" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="11"/>
     </row>
-    <row r="62" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="11"/>
     </row>
-    <row r="63" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="11"/>
     </row>
-    <row r="64" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="11"/>
     </row>
-    <row r="65" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="11"/>
     </row>
-    <row r="66" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="11"/>
     </row>
-    <row r="67" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="11"/>
     </row>
-    <row r="68" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="11"/>
     </row>
-    <row r="69" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="11"/>
     </row>
-    <row r="70" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C70" s="11"/>
     </row>
-    <row r="71" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="11"/>
     </row>
-    <row r="72" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="11"/>
     </row>
-    <row r="73" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C73" s="11"/>
     </row>
-    <row r="74" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C74" s="11"/>
     </row>
-    <row r="75" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C75" s="11"/>
     </row>
-    <row r="76" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C76" s="11"/>
     </row>
-    <row r="77" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C77" s="11"/>
     </row>
-    <row r="78" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C78" s="11"/>
     </row>
-    <row r="79" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C79" s="11"/>
     </row>
-    <row r="80" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C80" s="11"/>
     </row>
-    <row r="81" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C81" s="11"/>
     </row>
-    <row r="82" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C82" s="11"/>
     </row>
-    <row r="83" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C83" s="11"/>
     </row>
-    <row r="84" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C84" s="11"/>
     </row>
-    <row r="85" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C85" s="11"/>
     </row>
-    <row r="86" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C86" s="11"/>
     </row>
-    <row r="87" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C87" s="11"/>
     </row>
-    <row r="88" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C88" s="11"/>
     </row>
-    <row r="89" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C89" s="11"/>
     </row>
-    <row r="90" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C90" s="11"/>
     </row>
-    <row r="91" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C91" s="11"/>
     </row>
-    <row r="92" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C92" s="11"/>
     </row>
-    <row r="93" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C93" s="11"/>
     </row>
-    <row r="94" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C94" s="11"/>
     </row>
-    <row r="95" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C95" s="11"/>
     </row>
-    <row r="96" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C96" s="11"/>
     </row>
-    <row r="97" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C97" s="11"/>
     </row>
-    <row r="98" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C98" s="11"/>
     </row>
-    <row r="99" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C99" s="11"/>
     </row>
-    <row r="100" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C100" s="11"/>
     </row>
-    <row r="101" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C101" s="11"/>
     </row>
-    <row r="102" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C102" s="11"/>
     </row>
-    <row r="103" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C103" s="11"/>
     </row>
-    <row r="104" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C104" s="11"/>
     </row>
-    <row r="105" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C105" s="11"/>
     </row>
-    <row r="106" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C106" s="11"/>
     </row>
-    <row r="107" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C107" s="11"/>
     </row>
-    <row r="108" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C108" s="11"/>
     </row>
-    <row r="109" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C109" s="11"/>
     </row>
-    <row r="110" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C110" s="11"/>
     </row>
-    <row r="111" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C111" s="11"/>
     </row>
-    <row r="112" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C112" s="11"/>
     </row>
-    <row r="113" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C113" s="11"/>
     </row>
-    <row r="114" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C114" s="11"/>
     </row>
-    <row r="115" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C115" s="11"/>
     </row>
-    <row r="116" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C116" s="11"/>
     </row>
-    <row r="117" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C117" s="11"/>
     </row>
-    <row r="118" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C118" s="11"/>
     </row>
-    <row r="119" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C119" s="11"/>
     </row>
-    <row r="120" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C120" s="11"/>
     </row>
-    <row r="121" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C121" s="11"/>
     </row>
-    <row r="122" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C122" s="11"/>
     </row>
-    <row r="123" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C123" s="11"/>
     </row>
-    <row r="124" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C124" s="11"/>
     </row>
-    <row r="125" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C125" s="11"/>
     </row>
-    <row r="126" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C126" s="11"/>
     </row>
-    <row r="127" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C127" s="11"/>
     </row>
-    <row r="128" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C128" s="11"/>
     </row>
-    <row r="129" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C129" s="11"/>
     </row>
-    <row r="130" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C130" s="11"/>
     </row>
-    <row r="131" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C131" s="11"/>
     </row>
-    <row r="132" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C132" s="11"/>
     </row>
-    <row r="133" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C133" s="11"/>
     </row>
-    <row r="134" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C134" s="11"/>
     </row>
-    <row r="135" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C135" s="11"/>
     </row>
-    <row r="136" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C136" s="11"/>
     </row>
-    <row r="137" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C137" s="11"/>
     </row>
-    <row r="138" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C138" s="11"/>
     </row>
-    <row r="139" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C139" s="11"/>
     </row>
-    <row r="140" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C140" s="11"/>
     </row>
-    <row r="141" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C141" s="11"/>
     </row>
-    <row r="142" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C142" s="11"/>
     </row>
-    <row r="143" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C143" s="11"/>
     </row>
-    <row r="144" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C144" s="11"/>
     </row>
-    <row r="145" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C145" s="11"/>
     </row>
-    <row r="146" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C146" s="11"/>
     </row>
-    <row r="147" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C147" s="11"/>
     </row>
-    <row r="148" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C148" s="11"/>
     </row>
-    <row r="149" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C149" s="11"/>
     </row>
-    <row r="150" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C150" s="11"/>
     </row>
-    <row r="151" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C151" s="11"/>
     </row>
-    <row r="152" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C152" s="11"/>
     </row>
-    <row r="153" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C153" s="11"/>
     </row>
-    <row r="154" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C154" s="11"/>
     </row>
-    <row r="155" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C155" s="11"/>
     </row>
-    <row r="156" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C156" s="11"/>
     </row>
-    <row r="157" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C157" s="11"/>
     </row>
-    <row r="158" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C158" s="11"/>
     </row>
-    <row r="159" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C159" s="11"/>
     </row>
-    <row r="160" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C160" s="11"/>
     </row>
-    <row r="161" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C161" s="11"/>
     </row>
-    <row r="162" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C162" s="11"/>
     </row>
-    <row r="163" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C163" s="11"/>
     </row>
-    <row r="164" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C164" s="11"/>
     </row>
-    <row r="165" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C165" s="11"/>
     </row>
-    <row r="166" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C166" s="11"/>
     </row>
-    <row r="167" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C167" s="11"/>
     </row>
-    <row r="168" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C168" s="11"/>
     </row>
-    <row r="169" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C169" s="11"/>
     </row>
-    <row r="170" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C170" s="11"/>
     </row>
-    <row r="171" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C171" s="11"/>
     </row>
-    <row r="172" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C172" s="11"/>
     </row>
-    <row r="173" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C173" s="11"/>
     </row>
-    <row r="174" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C174" s="11"/>
     </row>
-    <row r="175" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C175" s="11"/>
     </row>
-    <row r="176" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C176" s="11"/>
     </row>
-    <row r="177" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C177" s="11"/>
     </row>
-    <row r="178" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C178" s="11"/>
     </row>
-    <row r="179" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C179" s="11"/>
     </row>
-    <row r="180" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C180" s="11"/>
     </row>
-    <row r="181" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C181" s="11"/>
     </row>
-    <row r="182" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C182" s="11"/>
     </row>
-    <row r="183" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C183" s="11"/>
     </row>
-    <row r="184" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C184" s="11"/>
     </row>
-    <row r="185" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C185" s="11"/>
     </row>
-    <row r="186" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C186" s="11"/>
     </row>
-    <row r="187" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C187" s="11"/>
     </row>
-    <row r="188" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C188" s="11"/>
     </row>
-    <row r="189" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C189" s="11"/>
     </row>
-    <row r="190" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C190" s="11"/>
     </row>
-    <row r="191" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C191" s="11"/>
     </row>
-    <row r="192" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C192" s="11"/>
     </row>
-    <row r="193" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C193" s="11"/>
     </row>
-    <row r="194" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C194" s="11"/>
     </row>
-    <row r="195" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C195" s="11"/>
     </row>
-    <row r="196" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C196" s="11"/>
     </row>
-    <row r="197" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C197" s="11"/>
     </row>
-    <row r="198" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C198" s="11"/>
     </row>
-    <row r="199" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C199" s="11"/>
     </row>
-    <row r="200" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C200" s="11"/>
     </row>
-    <row r="201" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C201" s="11"/>
     </row>
-    <row r="202" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C202" s="11"/>
     </row>
-    <row r="203" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C203" s="11"/>
     </row>
-    <row r="204" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C204" s="11"/>
     </row>
-    <row r="205" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C205" s="11"/>
     </row>
-    <row r="206" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C206" s="11"/>
     </row>
-    <row r="207" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C207" s="11"/>
     </row>
-    <row r="208" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C208" s="11"/>
     </row>
-    <row r="209" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C209" s="11"/>
     </row>
-    <row r="210" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C210" s="11"/>
     </row>
-    <row r="211" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C211" s="11"/>
     </row>
-    <row r="212" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C212" s="11"/>
     </row>
-    <row r="213" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C213" s="11"/>
     </row>
-    <row r="214" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C214" s="11"/>
     </row>
-    <row r="215" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C215" s="11"/>
     </row>
-    <row r="216" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C216" s="11"/>
     </row>
-    <row r="217" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C217" s="11"/>
     </row>
-    <row r="218" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C218" s="11"/>
     </row>
-    <row r="219" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C219" s="11"/>
     </row>
-    <row r="220" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C220" s="11"/>
     </row>
-    <row r="221" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C221" s="11"/>
     </row>
-    <row r="222" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C222" s="11"/>
     </row>
-    <row r="223" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C223" s="11"/>
     </row>
-    <row r="224" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C224" s="11"/>
     </row>
-    <row r="225" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C225" s="11"/>
     </row>
-    <row r="226" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C226" s="11"/>
     </row>
-    <row r="227" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C227" s="11"/>
     </row>
-    <row r="228" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C228" s="11"/>
     </row>
-    <row r="229" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C229" s="11"/>
     </row>
-    <row r="230" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C230" s="11"/>
     </row>
-    <row r="231" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C231" s="11"/>
     </row>
-    <row r="232" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C232" s="11"/>
     </row>
-    <row r="233" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C233" s="11"/>
     </row>
-    <row r="234" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C234" s="11"/>
     </row>
-    <row r="235" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C235" s="11"/>
     </row>
-    <row r="236" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C236" s="11"/>
     </row>
-    <row r="237" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C237" s="11"/>
     </row>
-    <row r="238" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C238" s="11"/>
     </row>
-    <row r="239" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C239" s="11"/>
     </row>
-    <row r="240" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C240" s="11"/>
     </row>
-    <row r="241" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C241" s="11"/>
     </row>
-    <row r="242" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C242" s="11"/>
     </row>
-    <row r="243" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C243" s="11"/>
     </row>
-    <row r="244" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C244" s="11"/>
     </row>
-    <row r="245" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C245" s="11"/>
     </row>
-    <row r="246" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C246" s="11"/>
     </row>
-    <row r="247" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C247" s="11"/>
     </row>
-    <row r="248" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C248" s="11"/>
     </row>
-    <row r="249" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C249" s="11"/>
     </row>
-    <row r="250" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C250" s="11"/>
     </row>
-    <row r="251" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C251" s="11"/>
     </row>
-    <row r="252" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C252" s="11"/>
     </row>
-    <row r="253" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C253" s="11"/>
     </row>
-    <row r="254" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C254" s="11"/>
     </row>
-    <row r="255" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C255" s="11"/>
     </row>
-    <row r="256" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C256" s="11"/>
     </row>
-    <row r="257" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C257" s="11"/>
     </row>
-    <row r="258" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C258" s="11"/>
     </row>
-    <row r="259" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C259" s="11"/>
     </row>
-    <row r="260" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C260" s="11"/>
     </row>
-    <row r="261" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C261" s="11"/>
     </row>
-    <row r="262" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C262" s="11"/>
     </row>
-    <row r="263" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C263" s="11"/>
     </row>
-    <row r="264" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C264" s="11"/>
     </row>
-    <row r="265" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C265" s="11"/>
     </row>
-    <row r="266" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C266" s="11"/>
     </row>
-    <row r="267" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C267" s="11"/>
     </row>
-    <row r="268" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C268" s="11"/>
     </row>
-    <row r="269" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C269" s="11"/>
     </row>
-    <row r="270" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C270" s="11"/>
     </row>
-    <row r="271" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C271" s="11"/>
     </row>
-    <row r="272" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C272" s="11"/>
     </row>
-    <row r="273" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C273" s="11"/>
     </row>
-    <row r="274" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C274" s="11"/>
     </row>
-    <row r="275" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C275" s="11"/>
     </row>
-    <row r="276" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C276" s="11"/>
     </row>
-    <row r="277" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C277" s="11"/>
     </row>
-    <row r="278" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C278" s="11"/>
     </row>
-    <row r="279" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C279" s="11"/>
     </row>
-    <row r="280" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C280" s="11"/>
     </row>
-    <row r="281" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C281" s="11"/>
     </row>
-    <row r="282" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C282" s="11"/>
     </row>
-    <row r="283" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C283" s="11"/>
     </row>
-    <row r="284" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C284" s="11"/>
     </row>
-    <row r="285" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C285" s="11"/>
     </row>
-    <row r="286" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C286" s="11"/>
     </row>
-    <row r="287" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C287" s="11"/>
     </row>
-    <row r="288" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C288" s="11"/>
     </row>
-    <row r="289" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C289" s="11"/>
     </row>
-    <row r="290" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C290" s="11"/>
     </row>
-    <row r="291" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C291" s="11"/>
     </row>
-    <row r="292" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C292" s="11"/>
     </row>
-    <row r="293" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C293" s="11"/>
     </row>
-    <row r="294" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C294" s="11"/>
     </row>
-    <row r="295" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C295" s="11"/>
     </row>
-    <row r="296" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C296" s="11"/>
     </row>
-    <row r="297" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C297" s="11"/>
     </row>
-    <row r="298" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C298" s="11"/>
     </row>
-    <row r="299" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C299" s="11"/>
     </row>
-    <row r="300" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C300" s="11"/>
     </row>
-    <row r="301" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C301" s="11"/>
     </row>
-    <row r="302" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C302" s="11"/>
     </row>
-    <row r="303" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C303" s="11"/>
     </row>
-    <row r="304" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C304" s="11"/>
     </row>
-    <row r="305" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C305" s="11"/>
     </row>
-    <row r="306" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C306" s="11"/>
     </row>
-    <row r="307" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C307" s="11"/>
     </row>
-    <row r="308" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C308" s="11"/>
     </row>
-    <row r="309" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C309" s="11"/>
     </row>
-    <row r="310" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C310" s="11"/>
     </row>
-    <row r="311" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C311" s="11"/>
     </row>
-    <row r="312" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C312" s="11"/>
     </row>
-    <row r="313" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C313" s="11"/>
     </row>
-    <row r="314" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C314" s="11"/>
     </row>
-    <row r="315" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C315" s="11"/>
     </row>
-    <row r="316" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C316" s="11"/>
     </row>
-    <row r="317" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C317" s="11"/>
     </row>
-    <row r="318" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C318" s="11"/>
     </row>
-    <row r="319" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C319" s="11"/>
     </row>
-    <row r="320" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C320" s="11"/>
     </row>
-    <row r="321" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C321" s="11"/>
     </row>
-    <row r="322" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C322" s="11"/>
     </row>
-    <row r="323" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C323" s="11"/>
     </row>
-    <row r="324" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C324" s="11"/>
     </row>
-    <row r="325" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C325" s="11"/>
     </row>
-    <row r="326" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C326" s="11"/>
     </row>
-    <row r="327" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C327" s="11"/>
     </row>
-    <row r="328" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C328" s="11"/>
     </row>
-    <row r="329" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C329" s="11"/>
     </row>
-    <row r="330" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C330" s="11"/>
     </row>
-    <row r="331" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C331" s="11"/>
     </row>
-    <row r="332" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C332" s="11"/>
     </row>
-    <row r="333" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C333" s="11"/>
     </row>
-    <row r="334" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C334" s="11"/>
     </row>
-    <row r="335" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C335" s="11"/>
     </row>
-    <row r="336" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C336" s="11"/>
     </row>
-    <row r="337" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C337" s="11"/>
     </row>
-    <row r="338" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C338" s="11"/>
     </row>
-    <row r="339" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C339" s="11"/>
     </row>
-    <row r="340" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C340" s="11"/>
     </row>
-    <row r="341" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C341" s="11"/>
     </row>
-    <row r="342" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C342" s="11"/>
     </row>
-    <row r="343" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C343" s="11"/>
     </row>
-    <row r="344" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C344" s="11"/>
     </row>
-    <row r="345" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C345" s="11"/>
     </row>
-    <row r="346" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C346" s="11"/>
     </row>
-    <row r="347" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C347" s="11"/>
     </row>
-    <row r="348" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C348" s="11"/>
     </row>
-    <row r="349" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C349" s="11"/>
     </row>
-    <row r="350" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C350" s="11"/>
     </row>
-    <row r="351" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C351" s="11"/>
     </row>
-    <row r="352" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C352" s="11"/>
     </row>
-    <row r="353" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C353" s="11"/>
     </row>
-    <row r="354" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C354" s="11"/>
     </row>
-    <row r="355" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C355" s="11"/>
     </row>
-    <row r="356" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C356" s="11"/>
     </row>
-    <row r="357" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C357" s="11"/>
     </row>
-    <row r="358" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C358" s="11"/>
     </row>
-    <row r="359" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C359" s="11"/>
     </row>
-    <row r="360" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C360" s="11"/>
     </row>
-    <row r="361" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C361" s="11"/>
     </row>
-    <row r="362" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C362" s="11"/>
     </row>
-    <row r="363" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C363" s="11"/>
     </row>
-    <row r="364" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C364" s="11"/>
     </row>
-    <row r="365" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C365" s="11"/>
     </row>
-    <row r="366" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C366" s="11"/>
     </row>
-    <row r="367" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C367" s="11"/>
     </row>
-    <row r="368" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C368" s="11"/>
     </row>
-    <row r="369" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C369" s="11"/>
     </row>
-    <row r="370" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C370" s="11"/>
     </row>
-    <row r="371" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C371" s="11"/>
     </row>
-    <row r="372" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C372" s="11"/>
     </row>
-    <row r="373" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C373" s="11"/>
     </row>
-    <row r="374" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C374" s="11"/>
     </row>
-    <row r="375" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C375" s="11"/>
     </row>
-    <row r="376" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C376" s="11"/>
     </row>
-    <row r="377" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C377" s="11"/>
     </row>
-    <row r="378" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C378" s="11"/>
     </row>
-    <row r="379" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C379" s="11"/>
     </row>
-    <row r="380" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C380" s="11"/>
     </row>
-    <row r="381" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C381" s="11"/>
     </row>
-    <row r="382" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C382" s="11"/>
     </row>
-    <row r="383" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C383" s="11"/>
     </row>
-    <row r="384" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C384" s="11"/>
     </row>
-    <row r="385" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C385" s="11"/>
     </row>
-    <row r="386" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C386" s="11"/>
     </row>
-    <row r="387" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C387" s="11"/>
     </row>
-    <row r="388" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C388" s="11"/>
     </row>
-    <row r="389" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C389" s="11"/>
     </row>
-    <row r="390" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C390" s="11"/>
     </row>
-    <row r="391" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C391" s="11"/>
     </row>
-    <row r="392" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C392" s="11"/>
     </row>
-    <row r="393" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C393" s="11"/>
     </row>
-    <row r="394" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C394" s="11"/>
     </row>
-    <row r="395" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C395" s="11"/>
     </row>
-    <row r="396" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C396" s="11"/>
     </row>
-    <row r="397" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C397" s="11"/>
     </row>
-    <row r="398" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C398" s="11"/>
     </row>
-    <row r="399" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C399" s="11"/>
     </row>
-    <row r="400" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C400" s="11"/>
     </row>
-    <row r="401" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="401" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C401" s="11"/>
     </row>
-    <row r="402" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="402" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C402" s="11"/>
     </row>
-    <row r="403" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="403" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C403" s="11"/>
     </row>
-    <row r="404" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C404" s="11"/>
     </row>
-    <row r="405" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C405" s="11"/>
     </row>
-    <row r="406" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C406" s="11"/>
     </row>
-    <row r="407" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C407" s="11"/>
     </row>
-    <row r="408" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C408" s="11"/>
     </row>
-    <row r="409" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C409" s="11"/>
     </row>
-    <row r="410" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="410" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C410" s="11"/>
     </row>
-    <row r="411" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="411" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C411" s="11"/>
     </row>
-    <row r="412" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="412" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C412" s="11"/>
     </row>
-    <row r="413" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="413" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C413" s="11"/>
     </row>
-    <row r="414" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="414" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C414" s="11"/>
     </row>
-    <row r="415" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="415" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C415" s="11"/>
     </row>
-    <row r="416" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="416" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C416" s="11"/>
     </row>
-    <row r="417" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C417" s="11"/>
     </row>
-    <row r="418" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C418" s="11"/>
     </row>
-    <row r="419" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C419" s="11"/>
     </row>
-    <row r="420" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C420" s="11"/>
     </row>
-    <row r="421" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C421" s="11"/>
     </row>
-    <row r="422" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C422" s="11"/>
     </row>
-    <row r="423" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C423" s="11"/>
     </row>
-    <row r="424" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="424" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C424" s="11"/>
     </row>
-    <row r="425" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="425" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C425" s="11"/>
     </row>
-    <row r="426" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C426" s="11"/>
     </row>
-    <row r="427" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C427" s="11"/>
     </row>
-    <row r="428" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C428" s="11"/>
     </row>
-    <row r="429" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="429" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C429" s="11"/>
     </row>
-    <row r="430" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="430" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C430" s="11"/>
     </row>
-    <row r="431" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="431" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C431" s="11"/>
     </row>
-    <row r="432" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="432" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C432" s="11"/>
     </row>
-    <row r="433" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="433" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C433" s="11"/>
     </row>
-    <row r="434" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="434" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C434" s="11"/>
     </row>
-    <row r="435" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="435" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C435" s="11"/>
     </row>
-    <row r="436" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C436" s="11"/>
     </row>
-    <row r="437" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="437" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C437" s="11"/>
     </row>
-    <row r="438" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="438" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C438" s="11"/>
     </row>
-    <row r="439" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C439" s="11"/>
     </row>
-    <row r="440" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C440" s="11"/>
     </row>
-    <row r="441" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="441" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C441" s="11"/>
     </row>
-    <row r="442" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="442" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C442" s="11"/>
     </row>
-    <row r="443" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="443" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C443" s="11"/>
     </row>
-    <row r="444" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="444" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C444" s="11"/>
     </row>
-    <row r="445" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="445" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C445" s="11"/>
     </row>
-    <row r="446" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="446" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C446" s="11"/>
     </row>
-    <row r="447" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="447" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C447" s="11"/>
     </row>
-    <row r="448" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="448" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C448" s="11"/>
     </row>
-    <row r="449" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="449" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C449" s="11"/>
     </row>
-    <row r="450" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="450" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C450" s="11"/>
     </row>
-    <row r="451" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="451" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C451" s="11"/>
     </row>
-    <row r="452" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="452" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C452" s="11"/>
     </row>
-    <row r="453" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="453" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C453" s="11"/>
     </row>
-    <row r="454" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="454" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C454" s="11"/>
     </row>
-    <row r="455" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="455" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C455" s="11"/>
     </row>
-    <row r="456" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="456" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C456" s="11"/>
     </row>
-    <row r="457" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="457" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C457" s="11"/>
     </row>
-    <row r="458" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="458" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C458" s="11"/>
     </row>
-    <row r="459" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="459" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C459" s="11"/>
     </row>
-    <row r="460" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="460" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C460" s="11"/>
     </row>
-    <row r="461" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="461" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C461" s="11"/>
     </row>
-    <row r="462" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="462" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C462" s="11"/>
     </row>
-    <row r="463" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="463" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C463" s="11"/>
     </row>
-    <row r="464" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="464" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C464" s="11"/>
     </row>
-    <row r="465" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="465" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C465" s="11"/>
     </row>
-    <row r="466" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="466" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C466" s="11"/>
     </row>
-    <row r="467" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="467" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C467" s="11"/>
     </row>
-    <row r="468" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="468" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C468" s="11"/>
     </row>
-    <row r="469" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="469" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C469" s="11"/>
     </row>
-    <row r="470" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="470" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C470" s="11"/>
     </row>
-    <row r="471" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="471" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C471" s="11"/>
     </row>
-    <row r="472" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="472" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C472" s="11"/>
     </row>
-    <row r="473" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="473" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C473" s="11"/>
     </row>
-    <row r="474" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="474" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C474" s="11"/>
     </row>
-    <row r="475" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="475" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C475" s="11"/>
     </row>
-    <row r="476" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="476" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C476" s="11"/>
     </row>
-    <row r="477" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="477" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C477" s="11"/>
     </row>
-    <row r="478" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="478" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C478" s="11"/>
     </row>
-    <row r="479" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="479" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C479" s="11"/>
     </row>
-    <row r="480" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="480" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C480" s="11"/>
     </row>
-    <row r="481" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="481" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C481" s="11"/>
     </row>
-    <row r="482" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="482" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C482" s="11"/>
     </row>
-    <row r="483" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="483" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C483" s="11"/>
     </row>
-    <row r="484" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="484" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C484" s="11"/>
     </row>
-    <row r="485" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="485" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C485" s="11"/>
     </row>
-    <row r="486" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="486" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C486" s="11"/>
     </row>
-    <row r="487" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="487" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C487" s="11"/>
     </row>
-    <row r="488" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="488" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C488" s="11"/>
     </row>
-    <row r="489" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="489" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C489" s="11"/>
     </row>
-    <row r="490" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="490" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C490" s="11"/>
     </row>
-    <row r="491" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="491" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C491" s="11"/>
     </row>
-    <row r="492" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="492" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C492" s="11"/>
     </row>
-    <row r="493" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="493" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C493" s="11"/>
     </row>
-    <row r="494" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="494" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C494" s="11"/>
     </row>
-    <row r="495" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="495" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C495" s="11"/>
     </row>
-    <row r="496" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="496" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C496" s="11"/>
     </row>
-    <row r="497" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="497" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C497" s="11"/>
     </row>
-    <row r="498" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="498" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C498" s="11"/>
     </row>
-    <row r="499" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="499" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C499" s="11"/>
     </row>
-    <row r="500" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="500" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C500" s="11"/>
     </row>
-    <row r="501" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="501" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C501" s="11"/>
     </row>
-    <row r="502" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="502" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C502" s="11"/>
     </row>
-    <row r="503" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="503" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C503" s="11"/>
     </row>
-    <row r="504" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="504" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C504" s="11"/>
     </row>
-    <row r="505" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="505" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C505" s="11"/>
     </row>
-    <row r="506" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="506" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C506" s="11"/>
     </row>
-    <row r="507" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="507" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C507" s="11"/>
     </row>
-    <row r="508" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="508" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C508" s="11"/>
     </row>
-    <row r="509" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="509" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C509" s="11"/>
     </row>
-    <row r="510" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="510" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C510" s="11"/>
     </row>
-    <row r="511" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="511" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C511" s="11"/>
     </row>
-    <row r="512" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="512" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C512" s="11"/>
     </row>
-    <row r="513" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="513" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C513" s="11"/>
     </row>
-    <row r="514" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="514" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C514" s="11"/>
     </row>
-    <row r="515" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="515" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C515" s="11"/>
     </row>
-    <row r="516" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="516" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C516" s="11"/>
     </row>
-    <row r="517" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="517" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C517" s="11"/>
     </row>
-    <row r="518" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="518" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C518" s="11"/>
     </row>
-    <row r="519" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="519" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C519" s="11"/>
     </row>
-    <row r="520" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="520" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C520" s="11"/>
     </row>
-    <row r="521" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="521" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C521" s="11"/>
     </row>
-    <row r="522" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="522" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C522" s="11"/>
     </row>
-    <row r="523" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="523" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C523" s="11"/>
     </row>
-    <row r="524" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="524" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C524" s="11"/>
     </row>
-    <row r="525" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="525" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C525" s="11"/>
     </row>
-    <row r="526" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="526" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C526" s="11"/>
     </row>
-    <row r="527" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="527" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C527" s="11"/>
     </row>
-    <row r="528" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="528" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C528" s="11"/>
     </row>
-    <row r="529" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="529" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C529" s="11"/>
     </row>
-    <row r="530" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="530" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C530" s="11"/>
     </row>
-    <row r="531" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="531" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C531" s="11"/>
     </row>
-    <row r="532" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="532" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C532" s="11"/>
     </row>
-    <row r="533" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="533" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C533" s="11"/>
     </row>
-    <row r="534" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="534" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C534" s="11"/>
     </row>
-    <row r="535" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="535" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C535" s="11"/>
     </row>
-    <row r="536" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="536" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C536" s="11"/>
     </row>
-    <row r="537" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="537" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C537" s="11"/>
     </row>
-    <row r="538" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="538" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C538" s="11"/>
     </row>
-    <row r="539" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="539" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C539" s="11"/>
     </row>
-    <row r="540" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="540" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C540" s="11"/>
     </row>
-    <row r="541" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="541" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C541" s="11"/>
     </row>
-    <row r="542" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="542" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C542" s="11"/>
     </row>
-    <row r="543" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="543" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C543" s="11"/>
     </row>
-    <row r="544" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="544" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C544" s="11"/>
     </row>
-    <row r="545" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="545" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C545" s="11"/>
     </row>
-    <row r="546" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="546" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C546" s="11"/>
     </row>
-    <row r="547" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="547" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C547" s="11"/>
     </row>
-    <row r="548" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="548" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C548" s="11"/>
     </row>
-    <row r="549" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="549" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C549" s="11"/>
     </row>
-    <row r="550" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="550" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C550" s="11"/>
     </row>
-    <row r="551" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="551" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C551" s="11"/>
     </row>
-    <row r="552" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="552" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C552" s="11"/>
     </row>
-    <row r="553" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="553" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C553" s="11"/>
     </row>
-    <row r="554" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="554" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C554" s="11"/>
     </row>
-    <row r="555" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="555" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C555" s="11"/>
     </row>
-    <row r="556" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="556" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C556" s="11"/>
     </row>
-    <row r="557" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="557" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C557" s="11"/>
     </row>
-    <row r="558" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="558" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C558" s="11"/>
     </row>
-    <row r="559" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="559" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C559" s="11"/>
     </row>
-    <row r="560" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="560" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C560" s="11"/>
     </row>
-    <row r="561" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="561" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C561" s="11"/>
     </row>
-    <row r="562" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="562" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C562" s="11"/>
     </row>
-    <row r="563" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="563" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C563" s="11"/>
     </row>
-    <row r="564" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="564" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C564" s="11"/>
     </row>
-    <row r="565" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="565" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C565" s="11"/>
     </row>
-    <row r="566" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="566" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C566" s="11"/>
     </row>
-    <row r="567" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="567" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C567" s="11"/>
     </row>
-    <row r="568" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="568" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C568" s="11"/>
     </row>
-    <row r="569" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="569" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C569" s="11"/>
     </row>
-    <row r="570" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="570" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C570" s="11"/>
     </row>
-    <row r="571" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="571" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C571" s="11"/>
     </row>
-    <row r="572" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="572" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C572" s="11"/>
     </row>
-    <row r="573" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="573" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C573" s="11"/>
     </row>
-    <row r="574" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="574" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C574" s="11"/>
     </row>
-    <row r="575" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="575" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C575" s="11"/>
     </row>
-    <row r="576" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="576" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C576" s="11"/>
     </row>
-    <row r="577" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="577" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C577" s="11"/>
     </row>
-    <row r="578" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="578" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C578" s="11"/>
     </row>
-    <row r="579" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="579" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C579" s="11"/>
     </row>
-    <row r="580" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="580" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C580" s="11"/>
     </row>
-    <row r="581" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="581" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C581" s="11"/>
     </row>
-    <row r="582" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="582" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C582" s="11"/>
     </row>
-    <row r="583" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="583" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C583" s="11"/>
     </row>
-    <row r="584" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="584" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C584" s="11"/>
     </row>
-    <row r="585" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="585" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C585" s="11"/>
     </row>
-    <row r="586" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="586" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C586" s="11"/>
     </row>
-    <row r="587" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="587" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C587" s="11"/>
     </row>
-    <row r="588" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="588" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C588" s="11"/>
     </row>
-    <row r="589" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="589" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C589" s="11"/>
     </row>
-    <row r="590" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="590" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C590" s="11"/>
     </row>
-    <row r="591" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="591" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C591" s="11"/>
     </row>
-    <row r="592" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="592" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C592" s="11"/>
     </row>
-    <row r="593" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="593" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C593" s="11"/>
     </row>
-    <row r="594" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="594" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C594" s="11"/>
     </row>
-    <row r="595" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="595" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C595" s="11"/>
     </row>
-    <row r="596" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="596" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C596" s="11"/>
     </row>
-    <row r="597" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="597" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C597" s="11"/>
     </row>
-    <row r="598" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="598" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C598" s="11"/>
     </row>
-    <row r="599" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="599" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C599" s="11"/>
     </row>
-    <row r="600" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="600" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C600" s="11"/>
     </row>
-    <row r="601" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="601" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C601" s="11"/>
     </row>
-    <row r="602" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="602" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C602" s="11"/>
     </row>
-    <row r="603" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="603" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C603" s="11"/>
     </row>
-    <row r="604" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="604" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C604" s="11"/>
     </row>
-    <row r="605" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="605" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C605" s="11"/>
     </row>
-    <row r="606" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="606" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C606" s="11"/>
     </row>
-    <row r="607" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="607" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C607" s="11"/>
     </row>
-    <row r="608" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="608" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C608" s="11"/>
     </row>
-    <row r="609" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="609" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C609" s="11"/>
     </row>
-    <row r="610" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="610" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C610" s="11"/>
     </row>
-    <row r="611" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="611" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C611" s="11"/>
     </row>
-    <row r="612" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="612" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C612" s="11"/>
     </row>
-    <row r="613" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="613" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C613" s="11"/>
     </row>
-    <row r="614" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="614" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C614" s="11"/>
     </row>
-    <row r="615" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="615" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C615" s="11"/>
     </row>
-    <row r="616" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="616" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C616" s="11"/>
     </row>
-    <row r="617" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="617" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C617" s="11"/>
     </row>
-    <row r="618" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="618" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C618" s="11"/>
     </row>
-    <row r="619" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="619" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C619" s="11"/>
     </row>
-    <row r="620" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="620" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C620" s="11"/>
     </row>
-    <row r="621" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="621" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C621" s="11"/>
     </row>
-    <row r="622" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="622" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C622" s="11"/>
     </row>
-    <row r="623" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="623" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C623" s="11"/>
     </row>
-    <row r="624" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="624" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C624" s="11"/>
     </row>
-    <row r="625" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="625" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C625" s="11"/>
     </row>
-    <row r="626" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="626" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C626" s="11"/>
     </row>
-    <row r="627" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="627" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C627" s="11"/>
     </row>
-    <row r="628" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="628" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C628" s="11"/>
     </row>
-    <row r="629" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="629" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C629" s="11"/>
     </row>
-    <row r="630" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="630" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C630" s="11"/>
     </row>
-    <row r="631" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="631" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C631" s="11"/>
     </row>
-    <row r="632" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="632" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C632" s="11"/>
     </row>
-    <row r="633" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="633" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C633" s="11"/>
     </row>
-    <row r="634" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="634" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C634" s="11"/>
     </row>
-    <row r="635" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="635" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C635" s="11"/>
     </row>
-    <row r="636" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="636" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C636" s="11"/>
     </row>
-    <row r="637" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="637" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C637" s="11"/>
     </row>
-    <row r="638" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="638" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C638" s="11"/>
     </row>
-    <row r="639" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="639" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C639" s="11"/>
     </row>
-    <row r="640" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="640" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C640" s="11"/>
     </row>
-    <row r="641" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="641" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C641" s="11"/>
     </row>
-    <row r="642" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="642" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C642" s="11"/>
     </row>
-    <row r="643" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="643" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C643" s="11"/>
     </row>
-    <row r="644" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="644" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C644" s="11"/>
     </row>
-    <row r="645" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="645" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C645" s="11"/>
     </row>
-    <row r="646" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="646" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C646" s="11"/>
     </row>
-    <row r="647" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="647" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C647" s="11"/>
     </row>
-    <row r="648" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="648" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C648" s="11"/>
     </row>
-    <row r="649" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="649" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C649" s="11"/>
     </row>
-    <row r="650" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="650" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C650" s="11"/>
     </row>
-    <row r="651" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="651" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C651" s="11"/>
     </row>
-    <row r="652" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="652" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C652" s="11"/>
     </row>
-    <row r="653" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="653" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C653" s="11"/>
     </row>
-    <row r="654" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="654" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C654" s="11"/>
     </row>
-    <row r="655" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="655" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C655" s="11"/>
     </row>
-    <row r="656" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="656" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C656" s="11"/>
     </row>
-    <row r="657" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="657" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C657" s="11"/>
     </row>
-    <row r="658" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="658" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C658" s="11"/>
     </row>
-    <row r="659" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="659" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C659" s="11"/>
     </row>
-    <row r="660" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="660" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C660" s="11"/>
     </row>
-    <row r="661" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="661" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C661" s="11"/>
     </row>
-    <row r="662" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="662" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C662" s="11"/>
     </row>
-    <row r="663" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="663" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C663" s="11"/>
     </row>
-    <row r="664" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="664" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C664" s="11"/>
     </row>
-    <row r="665" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="665" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C665" s="11"/>
     </row>
-    <row r="666" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="666" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C666" s="11"/>
     </row>
-    <row r="667" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="667" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C667" s="11"/>
     </row>
-    <row r="668" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="668" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C668" s="11"/>
     </row>
-    <row r="669" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="669" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C669" s="11"/>
     </row>
-    <row r="670" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="670" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C670" s="11"/>
     </row>
-    <row r="671" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="671" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C671" s="11"/>
     </row>
-    <row r="672" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="672" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C672" s="11"/>
     </row>
-    <row r="673" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="673" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C673" s="11"/>
     </row>
-    <row r="674" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="674" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C674" s="11"/>
     </row>
-    <row r="675" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="675" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C675" s="11"/>
     </row>
-    <row r="676" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="676" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C676" s="11"/>
     </row>
-    <row r="677" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="677" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C677" s="11"/>
     </row>
-    <row r="678" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="678" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C678" s="11"/>
     </row>
-    <row r="679" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="679" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C679" s="11"/>
     </row>
-    <row r="680" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="680" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C680" s="11"/>
     </row>
-    <row r="681" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="681" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C681" s="11"/>
     </row>
-    <row r="682" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="682" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C682" s="11"/>
     </row>
-    <row r="683" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="683" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C683" s="11"/>
     </row>
-    <row r="684" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="684" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C684" s="11"/>
     </row>
-    <row r="685" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="685" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C685" s="11"/>
     </row>
-    <row r="686" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="686" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C686" s="11"/>
     </row>
-    <row r="687" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="687" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C687" s="11"/>
     </row>
-    <row r="688" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="688" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C688" s="11"/>
     </row>
-    <row r="689" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="689" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C689" s="11"/>
     </row>
-    <row r="690" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="690" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C690" s="11"/>
     </row>
-    <row r="691" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="691" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C691" s="11"/>
     </row>
-    <row r="692" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="692" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C692" s="11"/>
     </row>
-    <row r="693" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="693" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C693" s="11"/>
     </row>
-    <row r="694" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="694" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C694" s="11"/>
     </row>
-    <row r="695" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="695" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C695" s="11"/>
     </row>
-    <row r="696" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="696" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C696" s="11"/>
     </row>
-    <row r="697" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="697" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C697" s="11"/>
     </row>
-    <row r="698" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="698" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C698" s="11"/>
     </row>
-    <row r="699" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="699" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C699" s="11"/>
     </row>
-    <row r="700" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="700" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C700" s="11"/>
     </row>
-    <row r="701" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="701" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C701" s="11"/>
     </row>
-    <row r="702" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="702" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C702" s="11"/>
     </row>
-    <row r="703" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="703" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C703" s="11"/>
     </row>
-    <row r="704" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="704" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C704" s="11"/>
     </row>
-    <row r="705" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="705" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C705" s="11"/>
     </row>
-    <row r="706" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="706" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C706" s="11"/>
     </row>
-    <row r="707" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="707" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C707" s="11"/>
     </row>
-    <row r="708" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="708" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C708" s="11"/>
     </row>
-    <row r="709" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="709" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C709" s="11"/>
     </row>
-    <row r="710" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="710" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C710" s="11"/>
     </row>
-    <row r="711" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="711" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C711" s="11"/>
     </row>
-    <row r="712" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="712" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C712" s="11"/>
     </row>
-    <row r="713" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="713" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C713" s="11"/>
     </row>
-    <row r="714" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="714" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C714" s="11"/>
     </row>
-    <row r="715" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="715" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C715" s="11"/>
     </row>
-    <row r="716" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="716" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C716" s="11"/>
     </row>
-    <row r="717" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="717" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C717" s="11"/>
     </row>
-    <row r="718" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="718" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C718" s="11"/>
     </row>
-    <row r="719" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="719" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C719" s="11"/>
     </row>
-    <row r="720" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="720" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C720" s="11"/>
     </row>
-    <row r="721" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="721" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C721" s="11"/>
     </row>
-    <row r="722" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="722" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C722" s="11"/>
     </row>
-    <row r="723" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="723" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C723" s="11"/>
     </row>
-    <row r="724" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="724" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C724" s="11"/>
     </row>
-    <row r="725" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="725" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C725" s="11"/>
     </row>
-    <row r="726" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="726" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C726" s="11"/>
     </row>
-    <row r="727" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="727" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C727" s="11"/>
     </row>
-    <row r="728" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="728" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C728" s="11"/>
     </row>
-    <row r="729" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="729" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C729" s="11"/>
     </row>
-    <row r="730" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="730" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C730" s="11"/>
     </row>
-    <row r="731" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="731" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C731" s="11"/>
     </row>
-    <row r="732" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="732" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C732" s="11"/>
     </row>
-    <row r="733" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="733" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C733" s="11"/>
     </row>
-    <row r="734" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="734" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C734" s="11"/>
     </row>
-    <row r="735" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="735" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C735" s="11"/>
     </row>
-    <row r="736" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="736" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C736" s="11"/>
     </row>
-    <row r="737" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="737" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C737" s="11"/>
     </row>
-    <row r="738" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="738" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C738" s="11"/>
     </row>
-    <row r="739" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="739" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C739" s="11"/>
     </row>
-    <row r="740" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="740" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C740" s="11"/>
     </row>
-    <row r="741" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="741" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C741" s="11"/>
     </row>
-    <row r="742" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="742" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C742" s="11"/>
     </row>
-    <row r="743" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="743" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C743" s="11"/>
     </row>
-    <row r="744" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="744" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C744" s="11"/>
     </row>
-    <row r="745" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="745" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C745" s="11"/>
     </row>
-    <row r="746" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="746" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C746" s="11"/>
     </row>
-    <row r="747" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="747" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C747" s="11"/>
     </row>
-    <row r="748" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="748" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C748" s="11"/>
     </row>
-    <row r="749" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="749" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C749" s="11"/>
     </row>
-    <row r="750" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="750" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C750" s="11"/>
     </row>
-    <row r="751" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="751" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C751" s="11"/>
     </row>
-    <row r="752" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="752" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C752" s="11"/>
     </row>
-    <row r="753" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="753" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C753" s="11"/>
     </row>
-    <row r="754" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="754" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C754" s="11"/>
     </row>
-    <row r="755" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="755" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C755" s="11"/>
     </row>
-    <row r="756" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="756" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C756" s="11"/>
     </row>
-    <row r="757" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="757" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C757" s="11"/>
     </row>
-    <row r="758" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="758" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C758" s="11"/>
     </row>
-    <row r="759" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="759" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C759" s="11"/>
     </row>
-    <row r="760" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="760" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C760" s="11"/>
     </row>
-    <row r="761" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="761" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C761" s="11"/>
     </row>
-    <row r="762" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="762" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C762" s="11"/>
     </row>
-    <row r="763" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="763" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C763" s="11"/>
     </row>
-    <row r="764" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="764" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C764" s="11"/>
     </row>
-    <row r="765" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="765" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C765" s="11"/>
     </row>
-    <row r="766" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="766" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C766" s="11"/>
     </row>
-    <row r="767" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="767" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C767" s="11"/>
     </row>
-    <row r="768" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="768" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C768" s="11"/>
     </row>
-    <row r="769" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="769" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C769" s="11"/>
     </row>
-    <row r="770" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="770" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C770" s="11"/>
     </row>
-    <row r="771" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="771" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C771" s="11"/>
     </row>
-    <row r="772" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="772" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C772" s="11"/>
     </row>
-    <row r="773" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="773" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C773" s="11"/>
     </row>
-    <row r="774" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="774" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C774" s="11"/>
     </row>
-    <row r="775" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="775" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C775" s="11"/>
     </row>
-    <row r="776" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="776" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C776" s="11"/>
     </row>
-    <row r="777" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="777" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C777" s="11"/>
     </row>
-    <row r="778" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="778" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C778" s="11"/>
     </row>
-    <row r="779" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="779" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C779" s="11"/>
     </row>
-    <row r="780" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="780" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C780" s="11"/>
     </row>
-    <row r="781" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="781" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C781" s="11"/>
     </row>
-    <row r="782" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="782" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C782" s="11"/>
     </row>
-    <row r="783" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="783" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C783" s="11"/>
     </row>
-    <row r="784" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="784" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C784" s="11"/>
     </row>
-    <row r="785" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="785" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C785" s="11"/>
     </row>
-    <row r="786" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="786" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C786" s="11"/>
     </row>
-    <row r="787" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="787" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C787" s="11"/>
     </row>
-    <row r="788" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="788" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C788" s="11"/>
     </row>
-    <row r="789" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="789" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C789" s="11"/>
     </row>
-    <row r="790" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="790" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C790" s="11"/>
     </row>
-    <row r="791" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="791" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C791" s="11"/>
     </row>
-    <row r="792" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="792" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C792" s="11"/>
     </row>
-    <row r="793" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="793" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C793" s="11"/>
     </row>
-    <row r="794" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="794" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C794" s="11"/>
     </row>
-    <row r="795" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="795" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C795" s="11"/>
     </row>
-    <row r="796" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="796" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C796" s="11"/>
     </row>
-    <row r="797" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="797" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C797" s="11"/>
     </row>
-    <row r="798" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="798" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C798" s="11"/>
     </row>
-    <row r="799" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="799" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C799" s="11"/>
     </row>
-    <row r="800" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="800" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C800" s="11"/>
     </row>
-    <row r="801" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="801" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C801" s="11"/>
     </row>
-    <row r="802" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="802" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C802" s="11"/>
     </row>
-    <row r="803" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="803" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C803" s="11"/>
     </row>
-    <row r="804" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="804" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C804" s="11"/>
     </row>
-    <row r="805" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="805" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C805" s="11"/>
     </row>
-    <row r="806" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="806" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C806" s="11"/>
     </row>
-    <row r="807" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="807" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C807" s="11"/>
     </row>
-    <row r="808" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="808" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C808" s="11"/>
     </row>
-    <row r="809" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="809" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C809" s="11"/>
     </row>
-    <row r="810" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="810" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C810" s="11"/>
     </row>
-    <row r="811" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="811" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C811" s="11"/>
     </row>
-    <row r="812" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="812" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C812" s="11"/>
     </row>
-    <row r="813" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="813" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C813" s="11"/>
     </row>
-    <row r="814" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="814" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C814" s="11"/>
     </row>
-    <row r="815" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="815" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C815" s="11"/>
     </row>
-    <row r="816" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="816" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C816" s="11"/>
     </row>
-    <row r="817" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="817" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C817" s="11"/>
     </row>
-    <row r="818" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="818" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C818" s="11"/>
     </row>
-    <row r="819" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="819" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C819" s="11"/>
     </row>
-    <row r="820" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="820" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C820" s="11"/>
     </row>
-    <row r="821" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="821" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C821" s="11"/>
     </row>
-    <row r="822" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="822" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C822" s="11"/>
     </row>
-    <row r="823" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="823" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C823" s="11"/>
     </row>
-    <row r="824" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="824" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C824" s="11"/>
     </row>
-    <row r="825" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="825" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C825" s="11"/>
     </row>
-    <row r="826" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="826" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C826" s="11"/>
     </row>
-    <row r="827" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="827" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C827" s="11"/>
     </row>
-    <row r="828" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="828" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C828" s="11"/>
     </row>
-    <row r="829" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="829" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C829" s="11"/>
     </row>
-    <row r="830" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="830" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C830" s="11"/>
     </row>
-    <row r="831" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="831" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C831" s="11"/>
     </row>
-    <row r="832" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="832" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C832" s="11"/>
     </row>
-    <row r="833" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="833" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C833" s="11"/>
     </row>
-    <row r="834" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="834" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C834" s="11"/>
     </row>
-    <row r="835" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="835" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C835" s="11"/>
     </row>
-    <row r="836" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="836" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C836" s="11"/>
     </row>
-    <row r="837" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="837" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C837" s="11"/>
     </row>
-    <row r="838" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="838" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C838" s="11"/>
     </row>
-    <row r="839" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="839" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C839" s="11"/>
     </row>
-    <row r="840" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="840" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C840" s="11"/>
     </row>
-    <row r="841" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="841" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C841" s="11"/>
     </row>
-    <row r="842" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="842" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C842" s="11"/>
     </row>
-    <row r="843" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="843" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C843" s="11"/>
     </row>
-    <row r="844" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="844" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C844" s="11"/>
     </row>
-    <row r="845" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="845" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C845" s="11"/>
     </row>
-    <row r="846" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="846" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C846" s="11"/>
     </row>
-    <row r="847" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="847" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C847" s="11"/>
     </row>
-    <row r="848" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="848" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C848" s="11"/>
     </row>
-    <row r="849" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="849" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C849" s="11"/>
     </row>
-    <row r="850" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="850" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C850" s="11"/>
     </row>
-    <row r="851" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="851" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C851" s="11"/>
     </row>
-    <row r="852" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="852" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C852" s="11"/>
     </row>
-    <row r="853" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="853" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C853" s="11"/>
     </row>
-    <row r="854" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="854" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C854" s="11"/>
     </row>
-    <row r="855" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="855" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C855" s="11"/>
     </row>
-    <row r="856" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="856" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C856" s="11"/>
     </row>
-    <row r="857" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="857" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C857" s="11"/>
     </row>
-    <row r="858" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="858" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C858" s="11"/>
     </row>
-    <row r="859" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="859" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C859" s="11"/>
     </row>
-    <row r="860" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="860" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C860" s="11"/>
     </row>
-    <row r="861" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="861" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C861" s="11"/>
     </row>
-    <row r="862" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="862" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C862" s="11"/>
     </row>
-    <row r="863" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="863" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C863" s="11"/>
     </row>
-    <row r="864" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="864" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C864" s="11"/>
     </row>
-    <row r="865" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="865" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C865" s="11"/>
     </row>
-    <row r="866" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="866" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C866" s="11"/>
     </row>
-    <row r="867" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="867" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C867" s="11"/>
     </row>
-    <row r="868" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="868" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C868" s="11"/>
     </row>
-    <row r="869" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="869" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C869" s="11"/>
     </row>
-    <row r="870" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="870" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C870" s="11"/>
     </row>
-    <row r="871" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="871" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C871" s="11"/>
     </row>
-    <row r="872" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="872" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C872" s="11"/>
     </row>
-    <row r="873" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="873" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C873" s="11"/>
     </row>
-    <row r="874" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="874" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C874" s="11"/>
     </row>
-    <row r="875" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="875" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C875" s="11"/>
     </row>
-    <row r="876" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="876" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C876" s="11"/>
     </row>
-    <row r="877" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="877" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C877" s="11"/>
     </row>
-    <row r="878" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="878" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C878" s="11"/>
     </row>
-    <row r="879" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="879" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C879" s="11"/>
     </row>
-    <row r="880" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="880" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C880" s="11"/>
     </row>
-    <row r="881" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="881" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C881" s="11"/>
     </row>
-    <row r="882" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="882" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C882" s="11"/>
     </row>
-    <row r="883" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="883" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C883" s="11"/>
     </row>
-    <row r="884" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="884" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C884" s="11"/>
     </row>
-    <row r="885" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="885" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C885" s="11"/>
     </row>
-    <row r="886" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="886" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C886" s="11"/>
     </row>
-    <row r="887" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="887" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C887" s="11"/>
     </row>
-    <row r="888" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="888" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C888" s="11"/>
     </row>
-    <row r="889" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="889" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C889" s="11"/>
     </row>
-    <row r="890" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="890" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C890" s="11"/>
     </row>
-    <row r="891" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="891" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C891" s="11"/>
     </row>
-    <row r="892" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="892" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C892" s="11"/>
     </row>
-    <row r="893" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="893" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C893" s="11"/>
     </row>
-    <row r="894" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="894" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C894" s="11"/>
     </row>
-    <row r="895" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="895" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C895" s="11"/>
     </row>
-    <row r="896" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="896" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C896" s="11"/>
     </row>
-    <row r="897" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="897" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C897" s="11"/>
     </row>
-    <row r="898" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="898" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C898" s="11"/>
     </row>
-    <row r="899" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="899" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C899" s="11"/>
     </row>
-    <row r="900" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="900" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C900" s="11"/>
     </row>
-    <row r="901" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="901" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C901" s="11"/>
     </row>
-    <row r="902" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="902" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C902" s="11"/>
     </row>
-    <row r="903" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="903" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C903" s="11"/>
     </row>
-    <row r="904" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="904" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C904" s="11"/>
     </row>
-    <row r="905" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="905" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C905" s="11"/>
     </row>
-    <row r="906" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="906" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C906" s="11"/>
     </row>
-    <row r="907" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="907" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C907" s="11"/>
     </row>
-    <row r="908" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="908" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C908" s="11"/>
     </row>
-    <row r="909" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="909" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C909" s="11"/>
     </row>
-    <row r="910" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="910" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C910" s="11"/>
     </row>
-    <row r="911" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="911" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C911" s="11"/>
     </row>
-    <row r="912" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="912" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C912" s="11"/>
     </row>
-    <row r="913" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="913" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C913" s="11"/>
     </row>
-    <row r="914" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="914" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C914" s="11"/>
     </row>
-    <row r="915" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="915" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C915" s="11"/>
     </row>
-    <row r="916" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="916" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C916" s="11"/>
     </row>
-    <row r="917" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="917" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C917" s="11"/>
     </row>
-    <row r="918" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="918" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C918" s="11"/>
     </row>
-    <row r="919" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="919" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C919" s="11"/>
     </row>
-    <row r="920" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="920" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C920" s="11"/>
     </row>
-    <row r="921" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="921" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C921" s="11"/>
     </row>
-    <row r="922" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="922" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C922" s="11"/>
     </row>
-    <row r="923" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="923" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C923" s="11"/>
     </row>
-    <row r="924" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="924" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C924" s="11"/>
     </row>
-    <row r="925" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="925" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C925" s="11"/>
     </row>
-    <row r="926" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="926" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C926" s="11"/>
     </row>
-    <row r="927" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="927" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C927" s="11"/>
     </row>
-    <row r="928" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="928" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C928" s="11"/>
     </row>
-    <row r="929" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="929" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C929" s="11"/>
     </row>
-    <row r="930" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="930" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C930" s="11"/>
     </row>
-    <row r="931" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="931" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C931" s="11"/>
     </row>
-    <row r="932" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="932" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C932" s="11"/>
     </row>
-    <row r="933" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="933" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C933" s="11"/>
     </row>
-    <row r="934" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="934" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C934" s="11"/>
     </row>
-    <row r="935" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="935" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C935" s="11"/>
     </row>
-    <row r="936" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="936" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C936" s="11"/>
     </row>
-    <row r="937" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="937" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C937" s="11"/>
     </row>
-    <row r="938" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="938" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C938" s="11"/>
     </row>
-    <row r="939" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="939" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C939" s="11"/>
     </row>
-    <row r="940" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="940" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C940" s="11"/>
     </row>
-    <row r="941" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="941" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C941" s="11"/>
     </row>
-    <row r="942" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="942" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C942" s="11"/>
     </row>
-    <row r="943" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="943" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C943" s="11"/>
     </row>
-    <row r="944" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="944" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C944" s="11"/>
     </row>
-    <row r="945" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="945" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C945" s="11"/>
     </row>
-    <row r="946" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="946" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C946" s="11"/>
     </row>
-    <row r="947" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="947" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C947" s="11"/>
     </row>
-    <row r="948" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="948" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C948" s="11"/>
     </row>
-    <row r="949" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="949" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C949" s="11"/>
     </row>
-    <row r="950" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="950" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C950" s="11"/>
     </row>
-    <row r="951" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="951" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C951" s="11"/>
     </row>
-    <row r="952" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="952" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C952" s="11"/>
     </row>
-    <row r="953" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="953" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C953" s="11"/>
     </row>
-    <row r="954" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="954" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C954" s="11"/>
     </row>
-    <row r="955" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="955" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C955" s="11"/>
     </row>
-    <row r="956" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="956" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C956" s="11"/>
     </row>
-    <row r="957" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="957" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C957" s="11"/>
     </row>
-    <row r="958" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="958" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C958" s="11"/>
     </row>
-    <row r="959" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="959" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C959" s="11"/>
     </row>
-    <row r="960" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="960" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C960" s="11"/>
     </row>
-    <row r="961" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="961" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C961" s="11"/>
     </row>
-    <row r="962" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="962" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C962" s="11"/>
     </row>
-    <row r="963" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="963" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C963" s="11"/>
     </row>
-    <row r="964" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="964" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C964" s="11"/>
     </row>
-    <row r="965" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="965" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C965" s="11"/>
     </row>
-    <row r="966" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="966" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C966" s="11"/>
     </row>
-    <row r="967" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="967" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C967" s="11"/>
     </row>
-    <row r="968" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="968" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C968" s="11"/>
     </row>
-    <row r="969" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="969" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C969" s="11"/>
     </row>
-    <row r="970" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="970" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C970" s="11"/>
     </row>
-    <row r="971" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="971" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C971" s="11"/>
     </row>
-    <row r="972" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="972" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C972" s="11"/>
     </row>
-    <row r="973" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="973" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C973" s="11"/>
     </row>
-    <row r="974" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="974" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C974" s="11"/>
     </row>
-    <row r="975" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="975" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C975" s="11"/>
     </row>
-    <row r="976" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="976" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C976" s="11"/>
     </row>
-    <row r="977" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="977" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C977" s="11"/>
     </row>
-    <row r="978" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="978" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C978" s="11"/>
     </row>
-    <row r="979" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="979" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C979" s="11"/>
     </row>
-    <row r="980" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="980" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C980" s="11"/>
     </row>
-    <row r="981" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="981" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C981" s="11"/>
     </row>
-    <row r="982" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="982" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C982" s="11"/>
     </row>
-    <row r="983" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="983" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C983" s="11"/>
     </row>
-    <row r="984" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="984" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C984" s="11"/>
     </row>
-    <row r="985" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="985" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C985" s="11"/>
     </row>
-    <row r="986" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="986" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C986" s="11"/>
     </row>
-    <row r="987" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="987" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C987" s="11"/>
     </row>
-    <row r="988" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="988" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C988" s="11"/>
     </row>
-    <row r="989" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="989" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C989" s="11"/>
     </row>
-    <row r="990" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="990" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C990" s="11"/>
     </row>
-    <row r="991" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="991" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C991" s="11"/>
     </row>
-    <row r="992" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="992" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C992" s="11"/>
     </row>
-    <row r="993" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="993" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C993" s="11"/>
     </row>
-    <row r="994" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="994" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C994" s="11"/>
     </row>
-    <row r="995" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="995" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C995" s="11"/>
     </row>
-    <row r="996" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="996" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C996" s="11"/>
     </row>
-    <row r="997" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="997" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C997" s="11"/>
     </row>
-    <row r="998" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="998" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C998" s="11"/>
     </row>
-    <row r="999" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="999" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C999" s="11"/>
     </row>
-    <row r="1000" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1000" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1000" s="11"/>
     </row>
-    <row r="1001" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1001" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1001" s="11"/>
     </row>
-    <row r="1002" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1002" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1002" s="11"/>
     </row>
-    <row r="1003" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1003" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1003" s="11"/>
     </row>
-    <row r="1004" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1004" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1004" s="11"/>
     </row>
-    <row r="1005" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1005" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1005" s="11"/>
     </row>
-    <row r="1006" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1006" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1006" s="11"/>
     </row>
-    <row r="1007" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1007" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1007" s="11"/>
     </row>
-    <row r="1008" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1008" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1008" s="11"/>
     </row>
-    <row r="1009" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1009" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1009" s="11"/>
     </row>
-    <row r="1010" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1010" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1010" s="11"/>
     </row>
-    <row r="1011" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1011" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1011" s="11"/>
     </row>
-    <row r="1012" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1012" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1012" s="11"/>
     </row>
-    <row r="1013" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1013" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1013" s="11"/>
     </row>
-    <row r="1014" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1014" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1014" s="11"/>
     </row>
-    <row r="1015" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1015" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1015" s="11"/>
     </row>
-    <row r="1016" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1016" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1016" s="11"/>
     </row>
-    <row r="1017" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1017" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1017" s="11"/>
     </row>
-    <row r="1018" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1018" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1018" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
@@ -4027,20 +4038,6 @@
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C1018" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Doc: updated according to coach comments
</commit_message>
<xml_diff>
--- a/Requirments/CRS-SIQ.xlsx
+++ b/Requirments/CRS-SIQ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI material\QA\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB8696E-0C0C-4CE4-9784-B232B8F56890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB55AEB5-5063-41EA-970B-EC9AB7041948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -148,11 +148,6 @@
     <t>CRS-SIQ_Client_003</t>
   </si>
   <si>
-    <t>order data in history of previous buys 
-1-format dd/mm/yy
-2-the date could not be future date</t>
-  </si>
-  <si>
     <t>CRS-SIQ_Client_004</t>
   </si>
   <si>
@@ -219,12 +214,6 @@
   </si>
   <si>
     <t xml:space="preserve">If the cart is empty, a message "Your cart is empty." shall be displayed. </t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>CRS-SIQ_Client_008</t>
   </si>
 </sst>
 </file>
@@ -409,14 +398,20 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -637,23 +632,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1019"/>
+  <dimension ref="A1:F1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="131.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="131.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="24.75" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,13 +658,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -679,11 +674,11 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -693,11 +688,11 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -707,11 +702,11 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -721,11 +716,11 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -735,11 +730,11 @@
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -749,11 +744,11 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -763,11 +758,11 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -777,11 +772,11 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -791,11 +786,11 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -805,11 +800,11 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -819,11 +814,11 @@
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -833,25 +828,25 @@
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -861,11 +856,11 @@
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
@@ -875,11 +870,11 @@
       <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -889,3169 +884,3165 @@
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="C31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C32" s="11"/>
     </row>
-    <row r="33" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C33" s="11"/>
     </row>
-    <row r="34" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C35" s="11"/>
     </row>
-    <row r="36" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C36" s="11"/>
     </row>
-    <row r="37" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C37" s="11"/>
     </row>
-    <row r="38" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C38" s="11"/>
     </row>
-    <row r="39" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C39" s="11"/>
     </row>
-    <row r="40" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C40" s="11"/>
     </row>
-    <row r="41" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C42" s="11"/>
     </row>
-    <row r="43" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C43" s="11"/>
     </row>
-    <row r="44" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C44" s="11"/>
     </row>
-    <row r="45" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="11"/>
     </row>
-    <row r="46" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="11"/>
     </row>
-    <row r="47" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="11"/>
     </row>
-    <row r="48" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="11"/>
     </row>
-    <row r="49" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="11"/>
     </row>
-    <row r="50" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="11"/>
     </row>
-    <row r="51" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="11"/>
     </row>
-    <row r="52" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="11"/>
     </row>
-    <row r="53" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="11"/>
     </row>
-    <row r="54" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="11"/>
     </row>
-    <row r="55" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="11"/>
     </row>
-    <row r="56" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="11"/>
     </row>
-    <row r="57" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="11"/>
     </row>
-    <row r="58" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="11"/>
     </row>
-    <row r="59" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="11"/>
     </row>
-    <row r="60" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="11"/>
     </row>
-    <row r="61" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="11"/>
     </row>
-    <row r="62" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="11"/>
     </row>
-    <row r="63" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="11"/>
     </row>
-    <row r="64" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="11"/>
     </row>
-    <row r="65" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="11"/>
     </row>
-    <row r="66" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="11"/>
     </row>
-    <row r="67" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="11"/>
     </row>
-    <row r="68" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="11"/>
     </row>
-    <row r="69" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="11"/>
     </row>
-    <row r="70" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C70" s="11"/>
     </row>
-    <row r="71" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="11"/>
     </row>
-    <row r="72" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="11"/>
     </row>
-    <row r="73" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C73" s="11"/>
     </row>
-    <row r="74" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C74" s="11"/>
     </row>
-    <row r="75" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C75" s="11"/>
     </row>
-    <row r="76" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C76" s="11"/>
     </row>
-    <row r="77" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C77" s="11"/>
     </row>
-    <row r="78" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C78" s="11"/>
     </row>
-    <row r="79" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C79" s="11"/>
     </row>
-    <row r="80" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C80" s="11"/>
     </row>
-    <row r="81" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C81" s="11"/>
     </row>
-    <row r="82" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C82" s="11"/>
     </row>
-    <row r="83" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C83" s="11"/>
     </row>
-    <row r="84" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C84" s="11"/>
     </row>
-    <row r="85" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C85" s="11"/>
     </row>
-    <row r="86" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C86" s="11"/>
     </row>
-    <row r="87" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C87" s="11"/>
     </row>
-    <row r="88" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C88" s="11"/>
     </row>
-    <row r="89" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C89" s="11"/>
     </row>
-    <row r="90" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C90" s="11"/>
     </row>
-    <row r="91" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C91" s="11"/>
     </row>
-    <row r="92" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C92" s="11"/>
     </row>
-    <row r="93" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C93" s="11"/>
     </row>
-    <row r="94" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C94" s="11"/>
     </row>
-    <row r="95" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C95" s="11"/>
     </row>
-    <row r="96" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C96" s="11"/>
     </row>
-    <row r="97" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C97" s="11"/>
     </row>
-    <row r="98" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C98" s="11"/>
     </row>
-    <row r="99" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C99" s="11"/>
     </row>
-    <row r="100" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C100" s="11"/>
     </row>
-    <row r="101" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C101" s="11"/>
     </row>
-    <row r="102" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C102" s="11"/>
     </row>
-    <row r="103" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C103" s="11"/>
     </row>
-    <row r="104" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C104" s="11"/>
     </row>
-    <row r="105" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C105" s="11"/>
     </row>
-    <row r="106" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C106" s="11"/>
     </row>
-    <row r="107" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C107" s="11"/>
     </row>
-    <row r="108" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C108" s="11"/>
     </row>
-    <row r="109" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C109" s="11"/>
     </row>
-    <row r="110" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C110" s="11"/>
     </row>
-    <row r="111" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C111" s="11"/>
     </row>
-    <row r="112" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C112" s="11"/>
     </row>
-    <row r="113" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C113" s="11"/>
     </row>
-    <row r="114" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C114" s="11"/>
     </row>
-    <row r="115" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C115" s="11"/>
     </row>
-    <row r="116" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C116" s="11"/>
     </row>
-    <row r="117" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C117" s="11"/>
     </row>
-    <row r="118" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C118" s="11"/>
     </row>
-    <row r="119" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C119" s="11"/>
     </row>
-    <row r="120" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C120" s="11"/>
     </row>
-    <row r="121" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C121" s="11"/>
     </row>
-    <row r="122" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C122" s="11"/>
     </row>
-    <row r="123" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C123" s="11"/>
     </row>
-    <row r="124" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C124" s="11"/>
     </row>
-    <row r="125" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C125" s="11"/>
     </row>
-    <row r="126" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C126" s="11"/>
     </row>
-    <row r="127" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C127" s="11"/>
     </row>
-    <row r="128" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C128" s="11"/>
     </row>
-    <row r="129" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C129" s="11"/>
     </row>
-    <row r="130" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C130" s="11"/>
     </row>
-    <row r="131" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C131" s="11"/>
     </row>
-    <row r="132" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C132" s="11"/>
     </row>
-    <row r="133" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C133" s="11"/>
     </row>
-    <row r="134" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C134" s="11"/>
     </row>
-    <row r="135" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C135" s="11"/>
     </row>
-    <row r="136" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C136" s="11"/>
     </row>
-    <row r="137" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C137" s="11"/>
     </row>
-    <row r="138" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C138" s="11"/>
     </row>
-    <row r="139" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C139" s="11"/>
     </row>
-    <row r="140" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C140" s="11"/>
     </row>
-    <row r="141" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C141" s="11"/>
     </row>
-    <row r="142" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C142" s="11"/>
     </row>
-    <row r="143" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C143" s="11"/>
     </row>
-    <row r="144" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C144" s="11"/>
     </row>
-    <row r="145" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C145" s="11"/>
     </row>
-    <row r="146" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C146" s="11"/>
     </row>
-    <row r="147" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C147" s="11"/>
     </row>
-    <row r="148" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C148" s="11"/>
     </row>
-    <row r="149" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C149" s="11"/>
     </row>
-    <row r="150" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C150" s="11"/>
     </row>
-    <row r="151" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C151" s="11"/>
     </row>
-    <row r="152" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C152" s="11"/>
     </row>
-    <row r="153" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C153" s="11"/>
     </row>
-    <row r="154" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C154" s="11"/>
     </row>
-    <row r="155" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C155" s="11"/>
     </row>
-    <row r="156" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C156" s="11"/>
     </row>
-    <row r="157" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C157" s="11"/>
     </row>
-    <row r="158" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C158" s="11"/>
     </row>
-    <row r="159" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C159" s="11"/>
     </row>
-    <row r="160" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C160" s="11"/>
     </row>
-    <row r="161" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C161" s="11"/>
     </row>
-    <row r="162" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C162" s="11"/>
     </row>
-    <row r="163" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C163" s="11"/>
     </row>
-    <row r="164" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C164" s="11"/>
     </row>
-    <row r="165" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C165" s="11"/>
     </row>
-    <row r="166" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C166" s="11"/>
     </row>
-    <row r="167" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C167" s="11"/>
     </row>
-    <row r="168" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C168" s="11"/>
     </row>
-    <row r="169" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C169" s="11"/>
     </row>
-    <row r="170" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C170" s="11"/>
     </row>
-    <row r="171" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C171" s="11"/>
     </row>
-    <row r="172" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C172" s="11"/>
     </row>
-    <row r="173" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C173" s="11"/>
     </row>
-    <row r="174" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C174" s="11"/>
     </row>
-    <row r="175" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C175" s="11"/>
     </row>
-    <row r="176" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C176" s="11"/>
     </row>
-    <row r="177" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C177" s="11"/>
     </row>
-    <row r="178" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C178" s="11"/>
     </row>
-    <row r="179" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C179" s="11"/>
     </row>
-    <row r="180" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C180" s="11"/>
     </row>
-    <row r="181" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C181" s="11"/>
     </row>
-    <row r="182" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C182" s="11"/>
     </row>
-    <row r="183" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C183" s="11"/>
     </row>
-    <row r="184" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C184" s="11"/>
     </row>
-    <row r="185" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C185" s="11"/>
     </row>
-    <row r="186" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C186" s="11"/>
     </row>
-    <row r="187" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C187" s="11"/>
     </row>
-    <row r="188" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C188" s="11"/>
     </row>
-    <row r="189" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C189" s="11"/>
     </row>
-    <row r="190" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C190" s="11"/>
     </row>
-    <row r="191" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C191" s="11"/>
     </row>
-    <row r="192" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C192" s="11"/>
     </row>
-    <row r="193" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C193" s="11"/>
     </row>
-    <row r="194" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C194" s="11"/>
     </row>
-    <row r="195" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C195" s="11"/>
     </row>
-    <row r="196" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C196" s="11"/>
     </row>
-    <row r="197" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C197" s="11"/>
     </row>
-    <row r="198" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C198" s="11"/>
     </row>
-    <row r="199" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C199" s="11"/>
     </row>
-    <row r="200" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C200" s="11"/>
     </row>
-    <row r="201" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C201" s="11"/>
     </row>
-    <row r="202" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C202" s="11"/>
     </row>
-    <row r="203" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C203" s="11"/>
     </row>
-    <row r="204" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C204" s="11"/>
     </row>
-    <row r="205" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C205" s="11"/>
     </row>
-    <row r="206" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C206" s="11"/>
     </row>
-    <row r="207" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C207" s="11"/>
     </row>
-    <row r="208" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C208" s="11"/>
     </row>
-    <row r="209" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C209" s="11"/>
     </row>
-    <row r="210" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C210" s="11"/>
     </row>
-    <row r="211" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C211" s="11"/>
     </row>
-    <row r="212" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C212" s="11"/>
     </row>
-    <row r="213" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C213" s="11"/>
     </row>
-    <row r="214" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C214" s="11"/>
     </row>
-    <row r="215" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C215" s="11"/>
     </row>
-    <row r="216" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C216" s="11"/>
     </row>
-    <row r="217" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C217" s="11"/>
     </row>
-    <row r="218" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C218" s="11"/>
     </row>
-    <row r="219" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C219" s="11"/>
     </row>
-    <row r="220" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C220" s="11"/>
     </row>
-    <row r="221" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C221" s="11"/>
     </row>
-    <row r="222" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C222" s="11"/>
     </row>
-    <row r="223" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C223" s="11"/>
     </row>
-    <row r="224" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C224" s="11"/>
     </row>
-    <row r="225" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C225" s="11"/>
     </row>
-    <row r="226" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C226" s="11"/>
     </row>
-    <row r="227" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C227" s="11"/>
     </row>
-    <row r="228" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C228" s="11"/>
     </row>
-    <row r="229" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C229" s="11"/>
     </row>
-    <row r="230" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C230" s="11"/>
     </row>
-    <row r="231" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C231" s="11"/>
     </row>
-    <row r="232" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C232" s="11"/>
     </row>
-    <row r="233" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C233" s="11"/>
     </row>
-    <row r="234" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C234" s="11"/>
     </row>
-    <row r="235" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C235" s="11"/>
     </row>
-    <row r="236" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C236" s="11"/>
     </row>
-    <row r="237" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C237" s="11"/>
     </row>
-    <row r="238" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C238" s="11"/>
     </row>
-    <row r="239" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C239" s="11"/>
     </row>
-    <row r="240" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C240" s="11"/>
     </row>
-    <row r="241" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C241" s="11"/>
     </row>
-    <row r="242" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C242" s="11"/>
     </row>
-    <row r="243" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C243" s="11"/>
     </row>
-    <row r="244" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C244" s="11"/>
     </row>
-    <row r="245" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C245" s="11"/>
     </row>
-    <row r="246" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C246" s="11"/>
     </row>
-    <row r="247" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C247" s="11"/>
     </row>
-    <row r="248" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C248" s="11"/>
     </row>
-    <row r="249" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C249" s="11"/>
     </row>
-    <row r="250" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C250" s="11"/>
     </row>
-    <row r="251" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C251" s="11"/>
     </row>
-    <row r="252" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C252" s="11"/>
     </row>
-    <row r="253" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C253" s="11"/>
     </row>
-    <row r="254" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C254" s="11"/>
     </row>
-    <row r="255" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C255" s="11"/>
     </row>
-    <row r="256" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C256" s="11"/>
     </row>
-    <row r="257" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C257" s="11"/>
     </row>
-    <row r="258" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C258" s="11"/>
     </row>
-    <row r="259" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C259" s="11"/>
     </row>
-    <row r="260" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C260" s="11"/>
     </row>
-    <row r="261" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C261" s="11"/>
     </row>
-    <row r="262" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C262" s="11"/>
     </row>
-    <row r="263" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C263" s="11"/>
     </row>
-    <row r="264" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C264" s="11"/>
     </row>
-    <row r="265" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C265" s="11"/>
     </row>
-    <row r="266" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C266" s="11"/>
     </row>
-    <row r="267" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C267" s="11"/>
     </row>
-    <row r="268" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C268" s="11"/>
     </row>
-    <row r="269" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C269" s="11"/>
     </row>
-    <row r="270" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C270" s="11"/>
     </row>
-    <row r="271" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C271" s="11"/>
     </row>
-    <row r="272" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C272" s="11"/>
     </row>
-    <row r="273" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C273" s="11"/>
     </row>
-    <row r="274" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C274" s="11"/>
     </row>
-    <row r="275" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C275" s="11"/>
     </row>
-    <row r="276" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C276" s="11"/>
     </row>
-    <row r="277" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C277" s="11"/>
     </row>
-    <row r="278" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C278" s="11"/>
     </row>
-    <row r="279" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C279" s="11"/>
     </row>
-    <row r="280" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C280" s="11"/>
     </row>
-    <row r="281" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C281" s="11"/>
     </row>
-    <row r="282" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C282" s="11"/>
     </row>
-    <row r="283" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C283" s="11"/>
     </row>
-    <row r="284" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C284" s="11"/>
     </row>
-    <row r="285" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C285" s="11"/>
     </row>
-    <row r="286" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C286" s="11"/>
     </row>
-    <row r="287" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C287" s="11"/>
     </row>
-    <row r="288" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C288" s="11"/>
     </row>
-    <row r="289" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C289" s="11"/>
     </row>
-    <row r="290" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C290" s="11"/>
     </row>
-    <row r="291" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C291" s="11"/>
     </row>
-    <row r="292" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C292" s="11"/>
     </row>
-    <row r="293" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C293" s="11"/>
     </row>
-    <row r="294" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C294" s="11"/>
     </row>
-    <row r="295" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C295" s="11"/>
     </row>
-    <row r="296" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C296" s="11"/>
     </row>
-    <row r="297" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C297" s="11"/>
     </row>
-    <row r="298" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C298" s="11"/>
     </row>
-    <row r="299" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C299" s="11"/>
     </row>
-    <row r="300" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C300" s="11"/>
     </row>
-    <row r="301" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C301" s="11"/>
     </row>
-    <row r="302" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C302" s="11"/>
     </row>
-    <row r="303" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C303" s="11"/>
     </row>
-    <row r="304" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C304" s="11"/>
     </row>
-    <row r="305" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C305" s="11"/>
     </row>
-    <row r="306" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C306" s="11"/>
     </row>
-    <row r="307" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C307" s="11"/>
     </row>
-    <row r="308" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C308" s="11"/>
     </row>
-    <row r="309" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C309" s="11"/>
     </row>
-    <row r="310" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C310" s="11"/>
     </row>
-    <row r="311" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C311" s="11"/>
     </row>
-    <row r="312" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C312" s="11"/>
     </row>
-    <row r="313" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C313" s="11"/>
     </row>
-    <row r="314" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C314" s="11"/>
     </row>
-    <row r="315" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C315" s="11"/>
     </row>
-    <row r="316" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C316" s="11"/>
     </row>
-    <row r="317" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C317" s="11"/>
     </row>
-    <row r="318" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C318" s="11"/>
     </row>
-    <row r="319" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C319" s="11"/>
     </row>
-    <row r="320" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C320" s="11"/>
     </row>
-    <row r="321" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C321" s="11"/>
     </row>
-    <row r="322" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C322" s="11"/>
     </row>
-    <row r="323" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C323" s="11"/>
     </row>
-    <row r="324" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C324" s="11"/>
     </row>
-    <row r="325" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C325" s="11"/>
     </row>
-    <row r="326" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C326" s="11"/>
     </row>
-    <row r="327" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C327" s="11"/>
     </row>
-    <row r="328" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C328" s="11"/>
     </row>
-    <row r="329" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C329" s="11"/>
     </row>
-    <row r="330" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C330" s="11"/>
     </row>
-    <row r="331" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C331" s="11"/>
     </row>
-    <row r="332" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C332" s="11"/>
     </row>
-    <row r="333" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C333" s="11"/>
     </row>
-    <row r="334" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C334" s="11"/>
     </row>
-    <row r="335" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C335" s="11"/>
     </row>
-    <row r="336" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C336" s="11"/>
     </row>
-    <row r="337" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C337" s="11"/>
     </row>
-    <row r="338" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C338" s="11"/>
     </row>
-    <row r="339" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C339" s="11"/>
     </row>
-    <row r="340" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C340" s="11"/>
     </row>
-    <row r="341" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C341" s="11"/>
     </row>
-    <row r="342" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C342" s="11"/>
     </row>
-    <row r="343" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C343" s="11"/>
     </row>
-    <row r="344" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C344" s="11"/>
     </row>
-    <row r="345" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C345" s="11"/>
     </row>
-    <row r="346" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C346" s="11"/>
     </row>
-    <row r="347" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C347" s="11"/>
     </row>
-    <row r="348" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C348" s="11"/>
     </row>
-    <row r="349" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C349" s="11"/>
     </row>
-    <row r="350" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C350" s="11"/>
     </row>
-    <row r="351" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C351" s="11"/>
     </row>
-    <row r="352" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C352" s="11"/>
     </row>
-    <row r="353" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C353" s="11"/>
     </row>
-    <row r="354" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C354" s="11"/>
     </row>
-    <row r="355" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C355" s="11"/>
     </row>
-    <row r="356" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C356" s="11"/>
     </row>
-    <row r="357" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C357" s="11"/>
     </row>
-    <row r="358" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C358" s="11"/>
     </row>
-    <row r="359" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C359" s="11"/>
     </row>
-    <row r="360" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C360" s="11"/>
     </row>
-    <row r="361" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C361" s="11"/>
     </row>
-    <row r="362" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C362" s="11"/>
     </row>
-    <row r="363" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C363" s="11"/>
     </row>
-    <row r="364" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C364" s="11"/>
     </row>
-    <row r="365" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C365" s="11"/>
     </row>
-    <row r="366" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C366" s="11"/>
     </row>
-    <row r="367" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C367" s="11"/>
     </row>
-    <row r="368" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C368" s="11"/>
     </row>
-    <row r="369" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C369" s="11"/>
     </row>
-    <row r="370" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C370" s="11"/>
     </row>
-    <row r="371" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C371" s="11"/>
     </row>
-    <row r="372" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C372" s="11"/>
     </row>
-    <row r="373" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C373" s="11"/>
     </row>
-    <row r="374" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C374" s="11"/>
     </row>
-    <row r="375" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C375" s="11"/>
     </row>
-    <row r="376" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C376" s="11"/>
     </row>
-    <row r="377" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C377" s="11"/>
     </row>
-    <row r="378" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C378" s="11"/>
     </row>
-    <row r="379" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C379" s="11"/>
     </row>
-    <row r="380" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C380" s="11"/>
     </row>
-    <row r="381" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C381" s="11"/>
     </row>
-    <row r="382" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C382" s="11"/>
     </row>
-    <row r="383" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C383" s="11"/>
     </row>
-    <row r="384" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C384" s="11"/>
     </row>
-    <row r="385" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C385" s="11"/>
     </row>
-    <row r="386" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C386" s="11"/>
     </row>
-    <row r="387" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C387" s="11"/>
     </row>
-    <row r="388" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C388" s="11"/>
     </row>
-    <row r="389" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C389" s="11"/>
     </row>
-    <row r="390" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C390" s="11"/>
     </row>
-    <row r="391" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C391" s="11"/>
     </row>
-    <row r="392" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C392" s="11"/>
     </row>
-    <row r="393" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C393" s="11"/>
     </row>
-    <row r="394" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C394" s="11"/>
     </row>
-    <row r="395" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C395" s="11"/>
     </row>
-    <row r="396" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C396" s="11"/>
     </row>
-    <row r="397" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C397" s="11"/>
     </row>
-    <row r="398" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C398" s="11"/>
     </row>
-    <row r="399" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C399" s="11"/>
     </row>
-    <row r="400" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C400" s="11"/>
     </row>
-    <row r="401" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="401" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C401" s="11"/>
     </row>
-    <row r="402" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="402" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C402" s="11"/>
     </row>
-    <row r="403" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="403" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C403" s="11"/>
     </row>
-    <row r="404" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C404" s="11"/>
     </row>
-    <row r="405" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C405" s="11"/>
     </row>
-    <row r="406" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C406" s="11"/>
     </row>
-    <row r="407" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C407" s="11"/>
     </row>
-    <row r="408" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C408" s="11"/>
     </row>
-    <row r="409" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C409" s="11"/>
     </row>
-    <row r="410" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="410" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C410" s="11"/>
     </row>
-    <row r="411" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="411" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C411" s="11"/>
     </row>
-    <row r="412" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="412" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C412" s="11"/>
     </row>
-    <row r="413" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="413" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C413" s="11"/>
     </row>
-    <row r="414" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="414" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C414" s="11"/>
     </row>
-    <row r="415" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="415" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C415" s="11"/>
     </row>
-    <row r="416" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="416" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C416" s="11"/>
     </row>
-    <row r="417" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C417" s="11"/>
     </row>
-    <row r="418" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C418" s="11"/>
     </row>
-    <row r="419" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C419" s="11"/>
     </row>
-    <row r="420" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C420" s="11"/>
     </row>
-    <row r="421" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C421" s="11"/>
     </row>
-    <row r="422" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C422" s="11"/>
     </row>
-    <row r="423" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C423" s="11"/>
     </row>
-    <row r="424" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="424" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C424" s="11"/>
     </row>
-    <row r="425" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="425" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C425" s="11"/>
     </row>
-    <row r="426" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C426" s="11"/>
     </row>
-    <row r="427" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C427" s="11"/>
     </row>
-    <row r="428" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C428" s="11"/>
     </row>
-    <row r="429" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="429" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C429" s="11"/>
     </row>
-    <row r="430" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="430" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C430" s="11"/>
     </row>
-    <row r="431" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="431" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C431" s="11"/>
     </row>
-    <row r="432" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="432" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C432" s="11"/>
     </row>
-    <row r="433" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="433" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C433" s="11"/>
     </row>
-    <row r="434" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="434" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C434" s="11"/>
     </row>
-    <row r="435" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="435" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C435" s="11"/>
     </row>
-    <row r="436" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C436" s="11"/>
     </row>
-    <row r="437" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="437" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C437" s="11"/>
     </row>
-    <row r="438" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="438" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C438" s="11"/>
     </row>
-    <row r="439" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C439" s="11"/>
     </row>
-    <row r="440" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C440" s="11"/>
     </row>
-    <row r="441" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="441" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C441" s="11"/>
     </row>
-    <row r="442" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="442" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C442" s="11"/>
     </row>
-    <row r="443" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="443" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C443" s="11"/>
     </row>
-    <row r="444" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="444" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C444" s="11"/>
     </row>
-    <row r="445" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="445" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C445" s="11"/>
     </row>
-    <row r="446" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="446" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C446" s="11"/>
     </row>
-    <row r="447" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="447" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C447" s="11"/>
     </row>
-    <row r="448" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="448" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C448" s="11"/>
     </row>
-    <row r="449" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="449" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C449" s="11"/>
     </row>
-    <row r="450" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="450" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C450" s="11"/>
     </row>
-    <row r="451" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="451" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C451" s="11"/>
     </row>
-    <row r="452" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="452" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C452" s="11"/>
     </row>
-    <row r="453" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="453" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C453" s="11"/>
     </row>
-    <row r="454" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="454" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C454" s="11"/>
     </row>
-    <row r="455" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="455" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C455" s="11"/>
     </row>
-    <row r="456" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="456" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C456" s="11"/>
     </row>
-    <row r="457" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="457" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C457" s="11"/>
     </row>
-    <row r="458" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="458" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C458" s="11"/>
     </row>
-    <row r="459" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="459" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C459" s="11"/>
     </row>
-    <row r="460" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="460" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C460" s="11"/>
     </row>
-    <row r="461" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="461" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C461" s="11"/>
     </row>
-    <row r="462" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="462" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C462" s="11"/>
     </row>
-    <row r="463" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="463" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C463" s="11"/>
     </row>
-    <row r="464" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="464" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C464" s="11"/>
     </row>
-    <row r="465" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="465" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C465" s="11"/>
     </row>
-    <row r="466" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="466" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C466" s="11"/>
     </row>
-    <row r="467" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="467" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C467" s="11"/>
     </row>
-    <row r="468" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="468" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C468" s="11"/>
     </row>
-    <row r="469" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="469" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C469" s="11"/>
     </row>
-    <row r="470" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="470" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C470" s="11"/>
     </row>
-    <row r="471" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="471" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C471" s="11"/>
     </row>
-    <row r="472" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="472" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C472" s="11"/>
     </row>
-    <row r="473" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="473" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C473" s="11"/>
     </row>
-    <row r="474" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="474" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C474" s="11"/>
     </row>
-    <row r="475" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="475" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C475" s="11"/>
     </row>
-    <row r="476" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="476" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C476" s="11"/>
     </row>
-    <row r="477" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="477" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C477" s="11"/>
     </row>
-    <row r="478" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="478" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C478" s="11"/>
     </row>
-    <row r="479" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="479" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C479" s="11"/>
     </row>
-    <row r="480" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="480" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C480" s="11"/>
     </row>
-    <row r="481" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="481" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C481" s="11"/>
     </row>
-    <row r="482" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="482" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C482" s="11"/>
     </row>
-    <row r="483" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="483" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C483" s="11"/>
     </row>
-    <row r="484" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="484" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C484" s="11"/>
     </row>
-    <row r="485" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="485" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C485" s="11"/>
     </row>
-    <row r="486" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="486" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C486" s="11"/>
     </row>
-    <row r="487" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="487" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C487" s="11"/>
     </row>
-    <row r="488" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="488" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C488" s="11"/>
     </row>
-    <row r="489" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="489" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C489" s="11"/>
     </row>
-    <row r="490" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="490" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C490" s="11"/>
     </row>
-    <row r="491" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="491" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C491" s="11"/>
     </row>
-    <row r="492" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="492" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C492" s="11"/>
     </row>
-    <row r="493" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="493" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C493" s="11"/>
     </row>
-    <row r="494" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="494" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C494" s="11"/>
     </row>
-    <row r="495" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="495" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C495" s="11"/>
     </row>
-    <row r="496" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="496" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C496" s="11"/>
     </row>
-    <row r="497" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="497" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C497" s="11"/>
     </row>
-    <row r="498" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="498" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C498" s="11"/>
     </row>
-    <row r="499" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="499" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C499" s="11"/>
     </row>
-    <row r="500" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="500" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C500" s="11"/>
     </row>
-    <row r="501" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="501" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C501" s="11"/>
     </row>
-    <row r="502" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="502" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C502" s="11"/>
     </row>
-    <row r="503" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="503" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C503" s="11"/>
     </row>
-    <row r="504" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="504" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C504" s="11"/>
     </row>
-    <row r="505" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="505" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C505" s="11"/>
     </row>
-    <row r="506" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="506" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C506" s="11"/>
     </row>
-    <row r="507" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="507" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C507" s="11"/>
     </row>
-    <row r="508" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="508" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C508" s="11"/>
     </row>
-    <row r="509" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="509" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C509" s="11"/>
     </row>
-    <row r="510" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="510" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C510" s="11"/>
     </row>
-    <row r="511" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="511" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C511" s="11"/>
     </row>
-    <row r="512" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="512" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C512" s="11"/>
     </row>
-    <row r="513" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="513" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C513" s="11"/>
     </row>
-    <row r="514" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="514" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C514" s="11"/>
     </row>
-    <row r="515" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="515" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C515" s="11"/>
     </row>
-    <row r="516" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="516" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C516" s="11"/>
     </row>
-    <row r="517" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="517" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C517" s="11"/>
     </row>
-    <row r="518" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="518" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C518" s="11"/>
     </row>
-    <row r="519" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="519" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C519" s="11"/>
     </row>
-    <row r="520" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="520" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C520" s="11"/>
     </row>
-    <row r="521" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="521" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C521" s="11"/>
     </row>
-    <row r="522" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="522" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C522" s="11"/>
     </row>
-    <row r="523" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="523" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C523" s="11"/>
     </row>
-    <row r="524" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="524" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C524" s="11"/>
     </row>
-    <row r="525" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="525" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C525" s="11"/>
     </row>
-    <row r="526" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="526" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C526" s="11"/>
     </row>
-    <row r="527" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="527" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C527" s="11"/>
     </row>
-    <row r="528" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="528" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C528" s="11"/>
     </row>
-    <row r="529" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="529" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C529" s="11"/>
     </row>
-    <row r="530" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="530" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C530" s="11"/>
     </row>
-    <row r="531" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="531" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C531" s="11"/>
     </row>
-    <row r="532" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="532" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C532" s="11"/>
     </row>
-    <row r="533" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="533" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C533" s="11"/>
     </row>
-    <row r="534" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="534" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C534" s="11"/>
     </row>
-    <row r="535" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="535" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C535" s="11"/>
     </row>
-    <row r="536" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="536" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C536" s="11"/>
     </row>
-    <row r="537" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="537" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C537" s="11"/>
     </row>
-    <row r="538" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="538" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C538" s="11"/>
     </row>
-    <row r="539" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="539" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C539" s="11"/>
     </row>
-    <row r="540" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="540" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C540" s="11"/>
     </row>
-    <row r="541" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="541" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C541" s="11"/>
     </row>
-    <row r="542" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="542" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C542" s="11"/>
     </row>
-    <row r="543" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="543" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C543" s="11"/>
     </row>
-    <row r="544" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="544" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C544" s="11"/>
     </row>
-    <row r="545" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="545" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C545" s="11"/>
     </row>
-    <row r="546" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="546" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C546" s="11"/>
     </row>
-    <row r="547" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="547" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C547" s="11"/>
     </row>
-    <row r="548" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="548" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C548" s="11"/>
     </row>
-    <row r="549" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="549" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C549" s="11"/>
     </row>
-    <row r="550" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="550" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C550" s="11"/>
     </row>
-    <row r="551" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="551" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C551" s="11"/>
     </row>
-    <row r="552" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="552" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C552" s="11"/>
     </row>
-    <row r="553" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="553" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C553" s="11"/>
     </row>
-    <row r="554" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="554" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C554" s="11"/>
     </row>
-    <row r="555" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="555" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C555" s="11"/>
     </row>
-    <row r="556" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="556" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C556" s="11"/>
     </row>
-    <row r="557" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="557" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C557" s="11"/>
     </row>
-    <row r="558" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="558" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C558" s="11"/>
     </row>
-    <row r="559" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="559" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C559" s="11"/>
     </row>
-    <row r="560" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="560" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C560" s="11"/>
     </row>
-    <row r="561" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="561" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C561" s="11"/>
     </row>
-    <row r="562" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="562" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C562" s="11"/>
     </row>
-    <row r="563" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="563" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C563" s="11"/>
     </row>
-    <row r="564" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="564" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C564" s="11"/>
     </row>
-    <row r="565" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="565" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C565" s="11"/>
     </row>
-    <row r="566" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="566" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C566" s="11"/>
     </row>
-    <row r="567" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="567" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C567" s="11"/>
     </row>
-    <row r="568" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="568" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C568" s="11"/>
     </row>
-    <row r="569" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="569" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C569" s="11"/>
     </row>
-    <row r="570" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="570" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C570" s="11"/>
     </row>
-    <row r="571" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="571" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C571" s="11"/>
     </row>
-    <row r="572" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="572" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C572" s="11"/>
     </row>
-    <row r="573" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="573" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C573" s="11"/>
     </row>
-    <row r="574" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="574" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C574" s="11"/>
     </row>
-    <row r="575" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="575" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C575" s="11"/>
     </row>
-    <row r="576" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="576" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C576" s="11"/>
     </row>
-    <row r="577" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="577" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C577" s="11"/>
     </row>
-    <row r="578" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="578" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C578" s="11"/>
     </row>
-    <row r="579" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="579" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C579" s="11"/>
     </row>
-    <row r="580" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="580" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C580" s="11"/>
     </row>
-    <row r="581" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="581" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C581" s="11"/>
     </row>
-    <row r="582" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="582" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C582" s="11"/>
     </row>
-    <row r="583" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="583" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C583" s="11"/>
     </row>
-    <row r="584" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="584" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C584" s="11"/>
     </row>
-    <row r="585" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="585" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C585" s="11"/>
     </row>
-    <row r="586" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="586" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C586" s="11"/>
     </row>
-    <row r="587" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="587" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C587" s="11"/>
     </row>
-    <row r="588" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="588" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C588" s="11"/>
     </row>
-    <row r="589" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="589" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C589" s="11"/>
     </row>
-    <row r="590" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="590" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C590" s="11"/>
     </row>
-    <row r="591" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="591" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C591" s="11"/>
     </row>
-    <row r="592" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="592" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C592" s="11"/>
     </row>
-    <row r="593" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="593" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C593" s="11"/>
     </row>
-    <row r="594" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="594" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C594" s="11"/>
     </row>
-    <row r="595" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="595" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C595" s="11"/>
     </row>
-    <row r="596" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="596" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C596" s="11"/>
     </row>
-    <row r="597" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="597" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C597" s="11"/>
     </row>
-    <row r="598" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="598" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C598" s="11"/>
     </row>
-    <row r="599" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="599" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C599" s="11"/>
     </row>
-    <row r="600" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="600" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C600" s="11"/>
     </row>
-    <row r="601" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="601" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C601" s="11"/>
     </row>
-    <row r="602" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="602" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C602" s="11"/>
     </row>
-    <row r="603" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="603" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C603" s="11"/>
     </row>
-    <row r="604" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="604" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C604" s="11"/>
     </row>
-    <row r="605" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="605" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C605" s="11"/>
     </row>
-    <row r="606" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="606" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C606" s="11"/>
     </row>
-    <row r="607" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="607" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C607" s="11"/>
     </row>
-    <row r="608" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="608" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C608" s="11"/>
     </row>
-    <row r="609" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="609" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C609" s="11"/>
     </row>
-    <row r="610" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="610" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C610" s="11"/>
     </row>
-    <row r="611" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="611" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C611" s="11"/>
     </row>
-    <row r="612" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="612" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C612" s="11"/>
     </row>
-    <row r="613" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="613" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C613" s="11"/>
     </row>
-    <row r="614" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="614" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C614" s="11"/>
     </row>
-    <row r="615" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="615" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C615" s="11"/>
     </row>
-    <row r="616" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="616" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C616" s="11"/>
     </row>
-    <row r="617" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="617" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C617" s="11"/>
     </row>
-    <row r="618" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="618" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C618" s="11"/>
     </row>
-    <row r="619" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="619" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C619" s="11"/>
     </row>
-    <row r="620" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="620" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C620" s="11"/>
     </row>
-    <row r="621" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="621" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C621" s="11"/>
     </row>
-    <row r="622" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="622" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C622" s="11"/>
     </row>
-    <row r="623" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="623" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C623" s="11"/>
     </row>
-    <row r="624" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="624" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C624" s="11"/>
     </row>
-    <row r="625" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="625" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C625" s="11"/>
     </row>
-    <row r="626" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="626" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C626" s="11"/>
     </row>
-    <row r="627" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="627" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C627" s="11"/>
     </row>
-    <row r="628" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="628" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C628" s="11"/>
     </row>
-    <row r="629" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="629" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C629" s="11"/>
     </row>
-    <row r="630" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="630" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C630" s="11"/>
     </row>
-    <row r="631" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="631" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C631" s="11"/>
     </row>
-    <row r="632" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="632" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C632" s="11"/>
     </row>
-    <row r="633" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="633" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C633" s="11"/>
     </row>
-    <row r="634" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="634" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C634" s="11"/>
     </row>
-    <row r="635" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="635" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C635" s="11"/>
     </row>
-    <row r="636" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="636" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C636" s="11"/>
     </row>
-    <row r="637" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="637" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C637" s="11"/>
     </row>
-    <row r="638" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="638" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C638" s="11"/>
     </row>
-    <row r="639" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="639" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C639" s="11"/>
     </row>
-    <row r="640" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="640" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C640" s="11"/>
     </row>
-    <row r="641" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="641" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C641" s="11"/>
     </row>
-    <row r="642" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="642" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C642" s="11"/>
     </row>
-    <row r="643" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="643" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C643" s="11"/>
     </row>
-    <row r="644" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="644" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C644" s="11"/>
     </row>
-    <row r="645" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="645" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C645" s="11"/>
     </row>
-    <row r="646" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="646" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C646" s="11"/>
     </row>
-    <row r="647" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="647" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C647" s="11"/>
     </row>
-    <row r="648" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="648" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C648" s="11"/>
     </row>
-    <row r="649" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="649" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C649" s="11"/>
     </row>
-    <row r="650" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="650" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C650" s="11"/>
     </row>
-    <row r="651" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="651" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C651" s="11"/>
     </row>
-    <row r="652" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="652" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C652" s="11"/>
     </row>
-    <row r="653" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="653" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C653" s="11"/>
     </row>
-    <row r="654" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="654" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C654" s="11"/>
     </row>
-    <row r="655" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="655" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C655" s="11"/>
     </row>
-    <row r="656" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="656" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C656" s="11"/>
     </row>
-    <row r="657" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="657" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C657" s="11"/>
     </row>
-    <row r="658" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="658" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C658" s="11"/>
     </row>
-    <row r="659" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="659" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C659" s="11"/>
     </row>
-    <row r="660" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="660" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C660" s="11"/>
     </row>
-    <row r="661" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="661" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C661" s="11"/>
     </row>
-    <row r="662" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="662" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C662" s="11"/>
     </row>
-    <row r="663" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="663" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C663" s="11"/>
     </row>
-    <row r="664" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="664" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C664" s="11"/>
     </row>
-    <row r="665" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="665" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C665" s="11"/>
     </row>
-    <row r="666" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="666" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C666" s="11"/>
     </row>
-    <row r="667" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="667" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C667" s="11"/>
     </row>
-    <row r="668" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="668" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C668" s="11"/>
     </row>
-    <row r="669" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="669" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C669" s="11"/>
     </row>
-    <row r="670" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="670" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C670" s="11"/>
     </row>
-    <row r="671" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="671" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C671" s="11"/>
     </row>
-    <row r="672" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="672" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C672" s="11"/>
     </row>
-    <row r="673" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="673" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C673" s="11"/>
     </row>
-    <row r="674" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="674" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C674" s="11"/>
     </row>
-    <row r="675" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="675" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C675" s="11"/>
     </row>
-    <row r="676" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="676" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C676" s="11"/>
     </row>
-    <row r="677" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="677" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C677" s="11"/>
     </row>
-    <row r="678" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="678" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C678" s="11"/>
     </row>
-    <row r="679" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="679" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C679" s="11"/>
     </row>
-    <row r="680" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="680" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C680" s="11"/>
     </row>
-    <row r="681" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="681" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C681" s="11"/>
     </row>
-    <row r="682" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="682" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C682" s="11"/>
     </row>
-    <row r="683" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="683" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C683" s="11"/>
     </row>
-    <row r="684" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="684" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C684" s="11"/>
     </row>
-    <row r="685" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="685" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C685" s="11"/>
     </row>
-    <row r="686" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="686" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C686" s="11"/>
     </row>
-    <row r="687" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="687" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C687" s="11"/>
     </row>
-    <row r="688" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="688" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C688" s="11"/>
     </row>
-    <row r="689" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="689" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C689" s="11"/>
     </row>
-    <row r="690" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="690" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C690" s="11"/>
     </row>
-    <row r="691" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="691" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C691" s="11"/>
     </row>
-    <row r="692" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="692" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C692" s="11"/>
     </row>
-    <row r="693" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="693" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C693" s="11"/>
     </row>
-    <row r="694" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="694" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C694" s="11"/>
     </row>
-    <row r="695" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="695" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C695" s="11"/>
     </row>
-    <row r="696" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="696" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C696" s="11"/>
     </row>
-    <row r="697" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="697" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C697" s="11"/>
     </row>
-    <row r="698" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="698" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C698" s="11"/>
     </row>
-    <row r="699" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="699" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C699" s="11"/>
     </row>
-    <row r="700" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="700" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C700" s="11"/>
     </row>
-    <row r="701" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="701" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C701" s="11"/>
     </row>
-    <row r="702" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="702" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C702" s="11"/>
     </row>
-    <row r="703" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="703" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C703" s="11"/>
     </row>
-    <row r="704" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="704" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C704" s="11"/>
     </row>
-    <row r="705" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="705" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C705" s="11"/>
     </row>
-    <row r="706" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="706" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C706" s="11"/>
     </row>
-    <row r="707" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="707" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C707" s="11"/>
     </row>
-    <row r="708" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="708" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C708" s="11"/>
     </row>
-    <row r="709" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="709" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C709" s="11"/>
     </row>
-    <row r="710" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="710" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C710" s="11"/>
     </row>
-    <row r="711" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="711" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C711" s="11"/>
     </row>
-    <row r="712" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="712" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C712" s="11"/>
     </row>
-    <row r="713" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="713" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C713" s="11"/>
     </row>
-    <row r="714" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="714" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C714" s="11"/>
     </row>
-    <row r="715" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="715" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C715" s="11"/>
     </row>
-    <row r="716" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="716" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C716" s="11"/>
     </row>
-    <row r="717" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="717" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C717" s="11"/>
     </row>
-    <row r="718" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="718" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C718" s="11"/>
     </row>
-    <row r="719" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="719" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C719" s="11"/>
     </row>
-    <row r="720" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="720" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C720" s="11"/>
     </row>
-    <row r="721" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="721" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C721" s="11"/>
     </row>
-    <row r="722" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="722" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C722" s="11"/>
     </row>
-    <row r="723" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="723" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C723" s="11"/>
     </row>
-    <row r="724" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="724" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C724" s="11"/>
     </row>
-    <row r="725" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="725" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C725" s="11"/>
     </row>
-    <row r="726" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="726" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C726" s="11"/>
     </row>
-    <row r="727" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="727" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C727" s="11"/>
     </row>
-    <row r="728" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="728" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C728" s="11"/>
     </row>
-    <row r="729" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="729" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C729" s="11"/>
     </row>
-    <row r="730" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="730" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C730" s="11"/>
     </row>
-    <row r="731" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="731" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C731" s="11"/>
     </row>
-    <row r="732" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="732" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C732" s="11"/>
     </row>
-    <row r="733" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="733" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C733" s="11"/>
     </row>
-    <row r="734" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="734" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C734" s="11"/>
     </row>
-    <row r="735" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="735" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C735" s="11"/>
     </row>
-    <row r="736" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="736" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C736" s="11"/>
     </row>
-    <row r="737" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="737" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C737" s="11"/>
     </row>
-    <row r="738" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="738" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C738" s="11"/>
     </row>
-    <row r="739" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="739" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C739" s="11"/>
     </row>
-    <row r="740" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="740" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C740" s="11"/>
     </row>
-    <row r="741" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="741" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C741" s="11"/>
     </row>
-    <row r="742" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="742" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C742" s="11"/>
     </row>
-    <row r="743" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="743" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C743" s="11"/>
     </row>
-    <row r="744" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="744" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C744" s="11"/>
     </row>
-    <row r="745" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="745" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C745" s="11"/>
     </row>
-    <row r="746" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="746" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C746" s="11"/>
     </row>
-    <row r="747" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="747" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C747" s="11"/>
     </row>
-    <row r="748" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="748" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C748" s="11"/>
     </row>
-    <row r="749" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="749" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C749" s="11"/>
     </row>
-    <row r="750" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="750" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C750" s="11"/>
     </row>
-    <row r="751" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="751" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C751" s="11"/>
     </row>
-    <row r="752" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="752" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C752" s="11"/>
     </row>
-    <row r="753" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="753" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C753" s="11"/>
     </row>
-    <row r="754" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="754" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C754" s="11"/>
     </row>
-    <row r="755" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="755" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C755" s="11"/>
     </row>
-    <row r="756" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="756" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C756" s="11"/>
     </row>
-    <row r="757" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="757" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C757" s="11"/>
     </row>
-    <row r="758" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="758" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C758" s="11"/>
     </row>
-    <row r="759" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="759" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C759" s="11"/>
     </row>
-    <row r="760" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="760" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C760" s="11"/>
     </row>
-    <row r="761" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="761" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C761" s="11"/>
     </row>
-    <row r="762" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="762" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C762" s="11"/>
     </row>
-    <row r="763" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="763" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C763" s="11"/>
     </row>
-    <row r="764" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="764" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C764" s="11"/>
     </row>
-    <row r="765" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="765" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C765" s="11"/>
     </row>
-    <row r="766" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="766" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C766" s="11"/>
     </row>
-    <row r="767" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="767" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C767" s="11"/>
     </row>
-    <row r="768" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="768" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C768" s="11"/>
     </row>
-    <row r="769" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="769" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C769" s="11"/>
     </row>
-    <row r="770" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="770" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C770" s="11"/>
     </row>
-    <row r="771" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="771" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C771" s="11"/>
     </row>
-    <row r="772" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="772" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C772" s="11"/>
     </row>
-    <row r="773" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="773" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C773" s="11"/>
     </row>
-    <row r="774" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="774" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C774" s="11"/>
     </row>
-    <row r="775" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="775" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C775" s="11"/>
     </row>
-    <row r="776" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="776" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C776" s="11"/>
     </row>
-    <row r="777" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="777" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C777" s="11"/>
     </row>
-    <row r="778" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="778" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C778" s="11"/>
     </row>
-    <row r="779" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="779" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C779" s="11"/>
     </row>
-    <row r="780" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="780" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C780" s="11"/>
     </row>
-    <row r="781" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="781" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C781" s="11"/>
     </row>
-    <row r="782" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="782" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C782" s="11"/>
     </row>
-    <row r="783" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="783" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C783" s="11"/>
     </row>
-    <row r="784" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="784" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C784" s="11"/>
     </row>
-    <row r="785" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="785" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C785" s="11"/>
     </row>
-    <row r="786" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="786" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C786" s="11"/>
     </row>
-    <row r="787" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="787" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C787" s="11"/>
     </row>
-    <row r="788" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="788" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C788" s="11"/>
     </row>
-    <row r="789" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="789" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C789" s="11"/>
     </row>
-    <row r="790" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="790" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C790" s="11"/>
     </row>
-    <row r="791" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="791" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C791" s="11"/>
     </row>
-    <row r="792" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="792" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C792" s="11"/>
     </row>
-    <row r="793" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="793" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C793" s="11"/>
     </row>
-    <row r="794" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="794" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C794" s="11"/>
     </row>
-    <row r="795" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="795" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C795" s="11"/>
     </row>
-    <row r="796" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="796" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C796" s="11"/>
     </row>
-    <row r="797" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="797" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C797" s="11"/>
     </row>
-    <row r="798" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="798" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C798" s="11"/>
     </row>
-    <row r="799" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="799" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C799" s="11"/>
     </row>
-    <row r="800" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="800" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C800" s="11"/>
     </row>
-    <row r="801" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="801" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C801" s="11"/>
     </row>
-    <row r="802" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="802" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C802" s="11"/>
     </row>
-    <row r="803" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="803" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C803" s="11"/>
     </row>
-    <row r="804" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="804" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C804" s="11"/>
     </row>
-    <row r="805" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="805" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C805" s="11"/>
     </row>
-    <row r="806" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="806" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C806" s="11"/>
     </row>
-    <row r="807" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="807" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C807" s="11"/>
     </row>
-    <row r="808" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="808" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C808" s="11"/>
     </row>
-    <row r="809" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="809" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C809" s="11"/>
     </row>
-    <row r="810" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="810" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C810" s="11"/>
     </row>
-    <row r="811" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="811" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C811" s="11"/>
     </row>
-    <row r="812" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="812" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C812" s="11"/>
     </row>
-    <row r="813" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="813" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C813" s="11"/>
     </row>
-    <row r="814" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="814" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C814" s="11"/>
     </row>
-    <row r="815" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="815" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C815" s="11"/>
     </row>
-    <row r="816" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="816" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C816" s="11"/>
     </row>
-    <row r="817" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="817" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C817" s="11"/>
     </row>
-    <row r="818" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="818" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C818" s="11"/>
     </row>
-    <row r="819" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="819" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C819" s="11"/>
     </row>
-    <row r="820" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="820" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C820" s="11"/>
     </row>
-    <row r="821" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="821" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C821" s="11"/>
     </row>
-    <row r="822" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="822" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C822" s="11"/>
     </row>
-    <row r="823" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="823" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C823" s="11"/>
     </row>
-    <row r="824" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="824" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C824" s="11"/>
     </row>
-    <row r="825" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="825" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C825" s="11"/>
     </row>
-    <row r="826" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="826" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C826" s="11"/>
     </row>
-    <row r="827" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="827" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C827" s="11"/>
     </row>
-    <row r="828" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="828" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C828" s="11"/>
     </row>
-    <row r="829" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="829" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C829" s="11"/>
     </row>
-    <row r="830" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="830" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C830" s="11"/>
     </row>
-    <row r="831" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="831" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C831" s="11"/>
     </row>
-    <row r="832" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="832" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C832" s="11"/>
     </row>
-    <row r="833" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="833" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C833" s="11"/>
     </row>
-    <row r="834" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="834" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C834" s="11"/>
     </row>
-    <row r="835" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="835" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C835" s="11"/>
     </row>
-    <row r="836" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="836" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C836" s="11"/>
     </row>
-    <row r="837" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="837" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C837" s="11"/>
     </row>
-    <row r="838" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="838" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C838" s="11"/>
     </row>
-    <row r="839" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="839" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C839" s="11"/>
     </row>
-    <row r="840" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="840" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C840" s="11"/>
     </row>
-    <row r="841" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="841" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C841" s="11"/>
     </row>
-    <row r="842" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="842" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C842" s="11"/>
     </row>
-    <row r="843" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="843" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C843" s="11"/>
     </row>
-    <row r="844" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="844" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C844" s="11"/>
     </row>
-    <row r="845" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="845" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C845" s="11"/>
     </row>
-    <row r="846" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="846" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C846" s="11"/>
     </row>
-    <row r="847" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="847" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C847" s="11"/>
     </row>
-    <row r="848" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="848" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C848" s="11"/>
     </row>
-    <row r="849" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="849" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C849" s="11"/>
     </row>
-    <row r="850" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="850" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C850" s="11"/>
     </row>
-    <row r="851" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="851" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C851" s="11"/>
     </row>
-    <row r="852" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="852" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C852" s="11"/>
     </row>
-    <row r="853" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="853" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C853" s="11"/>
     </row>
-    <row r="854" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="854" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C854" s="11"/>
     </row>
-    <row r="855" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="855" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C855" s="11"/>
     </row>
-    <row r="856" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="856" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C856" s="11"/>
     </row>
-    <row r="857" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="857" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C857" s="11"/>
     </row>
-    <row r="858" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="858" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C858" s="11"/>
     </row>
-    <row r="859" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="859" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C859" s="11"/>
     </row>
-    <row r="860" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="860" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C860" s="11"/>
     </row>
-    <row r="861" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="861" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C861" s="11"/>
     </row>
-    <row r="862" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="862" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C862" s="11"/>
     </row>
-    <row r="863" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="863" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C863" s="11"/>
     </row>
-    <row r="864" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="864" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C864" s="11"/>
     </row>
-    <row r="865" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="865" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C865" s="11"/>
     </row>
-    <row r="866" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="866" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C866" s="11"/>
     </row>
-    <row r="867" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="867" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C867" s="11"/>
     </row>
-    <row r="868" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="868" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C868" s="11"/>
     </row>
-    <row r="869" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="869" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C869" s="11"/>
     </row>
-    <row r="870" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="870" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C870" s="11"/>
     </row>
-    <row r="871" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="871" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C871" s="11"/>
     </row>
-    <row r="872" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="872" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C872" s="11"/>
     </row>
-    <row r="873" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="873" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C873" s="11"/>
     </row>
-    <row r="874" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="874" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C874" s="11"/>
     </row>
-    <row r="875" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="875" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C875" s="11"/>
     </row>
-    <row r="876" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="876" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C876" s="11"/>
     </row>
-    <row r="877" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="877" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C877" s="11"/>
     </row>
-    <row r="878" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="878" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C878" s="11"/>
     </row>
-    <row r="879" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="879" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C879" s="11"/>
     </row>
-    <row r="880" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="880" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C880" s="11"/>
     </row>
-    <row r="881" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="881" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C881" s="11"/>
     </row>
-    <row r="882" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="882" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C882" s="11"/>
     </row>
-    <row r="883" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="883" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C883" s="11"/>
     </row>
-    <row r="884" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="884" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C884" s="11"/>
     </row>
-    <row r="885" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="885" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C885" s="11"/>
     </row>
-    <row r="886" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="886" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C886" s="11"/>
     </row>
-    <row r="887" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="887" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C887" s="11"/>
     </row>
-    <row r="888" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="888" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C888" s="11"/>
     </row>
-    <row r="889" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="889" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C889" s="11"/>
     </row>
-    <row r="890" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="890" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C890" s="11"/>
     </row>
-    <row r="891" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="891" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C891" s="11"/>
     </row>
-    <row r="892" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="892" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C892" s="11"/>
     </row>
-    <row r="893" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="893" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C893" s="11"/>
     </row>
-    <row r="894" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="894" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C894" s="11"/>
     </row>
-    <row r="895" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="895" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C895" s="11"/>
     </row>
-    <row r="896" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="896" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C896" s="11"/>
     </row>
-    <row r="897" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="897" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C897" s="11"/>
     </row>
-    <row r="898" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="898" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C898" s="11"/>
     </row>
-    <row r="899" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="899" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C899" s="11"/>
     </row>
-    <row r="900" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="900" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C900" s="11"/>
     </row>
-    <row r="901" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="901" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C901" s="11"/>
     </row>
-    <row r="902" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="902" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C902" s="11"/>
     </row>
-    <row r="903" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="903" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C903" s="11"/>
     </row>
-    <row r="904" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="904" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C904" s="11"/>
     </row>
-    <row r="905" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="905" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C905" s="11"/>
     </row>
-    <row r="906" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="906" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C906" s="11"/>
     </row>
-    <row r="907" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="907" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C907" s="11"/>
     </row>
-    <row r="908" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="908" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C908" s="11"/>
     </row>
-    <row r="909" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="909" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C909" s="11"/>
     </row>
-    <row r="910" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="910" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C910" s="11"/>
     </row>
-    <row r="911" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="911" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C911" s="11"/>
     </row>
-    <row r="912" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="912" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C912" s="11"/>
     </row>
-    <row r="913" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="913" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C913" s="11"/>
     </row>
-    <row r="914" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="914" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C914" s="11"/>
     </row>
-    <row r="915" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="915" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C915" s="11"/>
     </row>
-    <row r="916" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="916" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C916" s="11"/>
     </row>
-    <row r="917" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="917" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C917" s="11"/>
     </row>
-    <row r="918" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="918" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C918" s="11"/>
     </row>
-    <row r="919" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="919" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C919" s="11"/>
     </row>
-    <row r="920" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="920" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C920" s="11"/>
     </row>
-    <row r="921" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="921" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C921" s="11"/>
     </row>
-    <row r="922" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="922" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C922" s="11"/>
     </row>
-    <row r="923" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="923" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C923" s="11"/>
     </row>
-    <row r="924" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="924" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C924" s="11"/>
     </row>
-    <row r="925" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="925" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C925" s="11"/>
     </row>
-    <row r="926" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="926" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C926" s="11"/>
     </row>
-    <row r="927" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="927" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C927" s="11"/>
     </row>
-    <row r="928" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="928" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C928" s="11"/>
     </row>
-    <row r="929" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="929" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C929" s="11"/>
     </row>
-    <row r="930" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="930" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C930" s="11"/>
     </row>
-    <row r="931" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="931" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C931" s="11"/>
     </row>
-    <row r="932" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="932" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C932" s="11"/>
     </row>
-    <row r="933" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="933" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C933" s="11"/>
     </row>
-    <row r="934" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="934" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C934" s="11"/>
     </row>
-    <row r="935" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="935" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C935" s="11"/>
     </row>
-    <row r="936" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="936" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C936" s="11"/>
     </row>
-    <row r="937" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="937" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C937" s="11"/>
     </row>
-    <row r="938" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="938" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C938" s="11"/>
     </row>
-    <row r="939" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="939" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C939" s="11"/>
     </row>
-    <row r="940" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="940" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C940" s="11"/>
     </row>
-    <row r="941" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="941" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C941" s="11"/>
     </row>
-    <row r="942" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="942" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C942" s="11"/>
     </row>
-    <row r="943" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="943" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C943" s="11"/>
     </row>
-    <row r="944" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="944" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C944" s="11"/>
     </row>
-    <row r="945" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="945" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C945" s="11"/>
     </row>
-    <row r="946" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="946" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C946" s="11"/>
     </row>
-    <row r="947" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="947" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C947" s="11"/>
     </row>
-    <row r="948" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="948" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C948" s="11"/>
     </row>
-    <row r="949" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="949" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C949" s="11"/>
     </row>
-    <row r="950" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="950" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C950" s="11"/>
     </row>
-    <row r="951" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="951" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C951" s="11"/>
     </row>
-    <row r="952" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="952" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C952" s="11"/>
     </row>
-    <row r="953" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="953" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C953" s="11"/>
     </row>
-    <row r="954" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="954" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C954" s="11"/>
     </row>
-    <row r="955" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="955" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C955" s="11"/>
     </row>
-    <row r="956" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="956" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C956" s="11"/>
     </row>
-    <row r="957" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="957" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C957" s="11"/>
     </row>
-    <row r="958" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="958" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C958" s="11"/>
     </row>
-    <row r="959" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="959" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C959" s="11"/>
     </row>
-    <row r="960" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="960" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C960" s="11"/>
     </row>
-    <row r="961" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="961" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C961" s="11"/>
     </row>
-    <row r="962" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="962" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C962" s="11"/>
     </row>
-    <row r="963" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="963" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C963" s="11"/>
     </row>
-    <row r="964" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="964" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C964" s="11"/>
     </row>
-    <row r="965" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="965" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C965" s="11"/>
     </row>
-    <row r="966" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="966" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C966" s="11"/>
     </row>
-    <row r="967" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="967" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C967" s="11"/>
     </row>
-    <row r="968" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="968" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C968" s="11"/>
     </row>
-    <row r="969" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="969" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C969" s="11"/>
     </row>
-    <row r="970" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="970" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C970" s="11"/>
     </row>
-    <row r="971" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="971" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C971" s="11"/>
     </row>
-    <row r="972" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="972" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C972" s="11"/>
     </row>
-    <row r="973" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="973" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C973" s="11"/>
     </row>
-    <row r="974" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="974" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C974" s="11"/>
     </row>
-    <row r="975" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="975" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C975" s="11"/>
     </row>
-    <row r="976" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="976" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C976" s="11"/>
     </row>
-    <row r="977" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="977" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C977" s="11"/>
     </row>
-    <row r="978" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="978" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C978" s="11"/>
     </row>
-    <row r="979" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="979" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C979" s="11"/>
     </row>
-    <row r="980" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="980" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C980" s="11"/>
     </row>
-    <row r="981" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="981" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C981" s="11"/>
     </row>
-    <row r="982" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="982" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C982" s="11"/>
     </row>
-    <row r="983" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="983" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C983" s="11"/>
     </row>
-    <row r="984" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="984" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C984" s="11"/>
     </row>
-    <row r="985" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="985" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C985" s="11"/>
     </row>
-    <row r="986" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="986" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C986" s="11"/>
     </row>
-    <row r="987" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="987" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C987" s="11"/>
     </row>
-    <row r="988" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="988" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C988" s="11"/>
     </row>
-    <row r="989" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="989" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C989" s="11"/>
     </row>
-    <row r="990" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="990" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C990" s="11"/>
     </row>
-    <row r="991" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="991" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C991" s="11"/>
     </row>
-    <row r="992" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="992" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C992" s="11"/>
     </row>
-    <row r="993" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="993" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C993" s="11"/>
     </row>
-    <row r="994" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="994" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C994" s="11"/>
     </row>
-    <row r="995" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="995" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C995" s="11"/>
     </row>
-    <row r="996" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="996" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C996" s="11"/>
     </row>
-    <row r="997" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="997" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C997" s="11"/>
     </row>
-    <row r="998" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="998" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C998" s="11"/>
     </row>
-    <row r="999" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="999" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C999" s="11"/>
     </row>
-    <row r="1000" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1000" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1000" s="11"/>
     </row>
-    <row r="1001" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1001" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1001" s="11"/>
     </row>
-    <row r="1002" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1002" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1002" s="11"/>
     </row>
-    <row r="1003" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1003" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1003" s="11"/>
     </row>
-    <row r="1004" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1004" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1004" s="11"/>
     </row>
-    <row r="1005" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1005" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1005" s="11"/>
     </row>
-    <row r="1006" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1006" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1006" s="11"/>
     </row>
-    <row r="1007" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1007" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1007" s="11"/>
     </row>
-    <row r="1008" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1008" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1008" s="11"/>
     </row>
-    <row r="1009" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1009" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1009" s="11"/>
     </row>
-    <row r="1010" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1010" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1010" s="11"/>
     </row>
-    <row r="1011" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1011" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1011" s="11"/>
     </row>
-    <row r="1012" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1012" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1012" s="11"/>
     </row>
-    <row r="1013" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1013" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1013" s="11"/>
     </row>
-    <row r="1014" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1014" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1014" s="11"/>
     </row>
-    <row r="1015" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1015" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1015" s="11"/>
     </row>
-    <row r="1016" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1016" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1016" s="11"/>
     </row>
-    <row r="1017" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1017" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1017" s="11"/>
     </row>
-    <row r="1018" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1018" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C1018" s="11"/>
     </row>
-    <row r="1019" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="C1019" s="11"/>
-    </row>
+    <row r="1019" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1020" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1021" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1022" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1023" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1024" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1025" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1026" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1027" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1028" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D3:F3"/>
@@ -4063,27 +4054,27 @@
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D30:F30"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D29:F29"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C1019" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C23 C24:C1018" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No,Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updating CRS-SIQ & CRS & SRS fro supplier feature
</commit_message>
<xml_diff>
--- a/Requirments/CRS-SIQ.xlsx
+++ b/Requirments/CRS-SIQ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB55AEB5-5063-41EA-970B-EC9AB7041948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F690F5E-E983-411E-8E22-713BDC4475DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -214,6 +214,24 @@
   </si>
   <si>
     <t xml:space="preserve">If the cart is empty, a message "Your cart is empty." shall be displayed. </t>
+  </si>
+  <si>
+    <t>CRS-SIQ_supplier_007</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_supplier_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the first filed that has an error will be highlighted by red color and exclamation mark appears in the right of the field </t>
+  </si>
+  <si>
+    <t>The product id should be unique, there are not two products with the same product id</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_supplier_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The error message,in red color,  appears in the top of the form of add product and update product </t>
   </si>
 </sst>
 </file>
@@ -319,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -379,11 +397,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -398,6 +425,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -635,20 +663,20 @@
   <dimension ref="A1:F1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="131.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="131.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="25.2" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,13 +686,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E1" s="15"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -674,11 +702,11 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -688,11 +716,11 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -702,11 +730,11 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -716,11 +744,11 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -730,11 +758,11 @@
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -744,11 +772,11 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -758,11 +786,11 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -772,11 +800,11 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -786,11 +814,11 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -800,11 +828,11 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -814,11 +842,11 @@
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -828,11 +856,11 @@
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -842,11 +870,11 @@
       <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -856,11 +884,11 @@
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
@@ -870,11 +898,11 @@
       <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -884,11 +912,11 @@
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
@@ -898,11 +926,11 @@
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -912,11 +940,11 @@
       <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
@@ -926,11 +954,11 @@
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
@@ -940,11 +968,11 @@
       <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
@@ -954,11 +982,11 @@
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>45</v>
       </c>
@@ -968,11 +996,11 @@
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-    </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>47</v>
       </c>
@@ -982,11 +1010,11 @@
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>49</v>
       </c>
@@ -996,11 +1024,11 @@
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
@@ -1010,11 +1038,11 @@
       <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D26" s="14"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
@@ -1024,11 +1052,11 @@
       <c r="C27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>55</v>
       </c>
@@ -1038,11 +1066,11 @@
       <c r="C28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>57</v>
       </c>
@@ -1052,2996 +1080,3010 @@
       <c r="C29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="C30" s="10"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+    </row>
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="C31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="C32" s="11"/>
     </row>
-    <row r="33" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C33" s="11"/>
     </row>
-    <row r="34" spans="3:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C35" s="11"/>
     </row>
-    <row r="36" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C36" s="11"/>
     </row>
-    <row r="37" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C37" s="11"/>
     </row>
-    <row r="38" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C38" s="11"/>
     </row>
-    <row r="39" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C39" s="11"/>
     </row>
-    <row r="40" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C40" s="11"/>
     </row>
-    <row r="41" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C42" s="11"/>
     </row>
-    <row r="43" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C43" s="11"/>
     </row>
-    <row r="44" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C44" s="11"/>
     </row>
-    <row r="45" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C45" s="11"/>
     </row>
-    <row r="46" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C46" s="11"/>
     </row>
-    <row r="47" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C47" s="11"/>
     </row>
-    <row r="48" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C48" s="11"/>
     </row>
-    <row r="49" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C49" s="11"/>
     </row>
-    <row r="50" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C50" s="11"/>
     </row>
-    <row r="51" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C51" s="11"/>
     </row>
-    <row r="52" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C52" s="11"/>
     </row>
-    <row r="53" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C53" s="11"/>
     </row>
-    <row r="54" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C54" s="11"/>
     </row>
-    <row r="55" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C55" s="11"/>
     </row>
-    <row r="56" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C56" s="11"/>
     </row>
-    <row r="57" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C57" s="11"/>
     </row>
-    <row r="58" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C58" s="11"/>
     </row>
-    <row r="59" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C59" s="11"/>
     </row>
-    <row r="60" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C60" s="11"/>
     </row>
-    <row r="61" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C61" s="11"/>
     </row>
-    <row r="62" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C62" s="11"/>
     </row>
-    <row r="63" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C63" s="11"/>
     </row>
-    <row r="64" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C64" s="11"/>
     </row>
-    <row r="65" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C65" s="11"/>
     </row>
-    <row r="66" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C66" s="11"/>
     </row>
-    <row r="67" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C67" s="11"/>
     </row>
-    <row r="68" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C68" s="11"/>
     </row>
-    <row r="69" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C69" s="11"/>
     </row>
-    <row r="70" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C70" s="11"/>
     </row>
-    <row r="71" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C71" s="11"/>
     </row>
-    <row r="72" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C72" s="11"/>
     </row>
-    <row r="73" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C73" s="11"/>
     </row>
-    <row r="74" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C74" s="11"/>
     </row>
-    <row r="75" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C75" s="11"/>
     </row>
-    <row r="76" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C76" s="11"/>
     </row>
-    <row r="77" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C77" s="11"/>
     </row>
-    <row r="78" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C78" s="11"/>
     </row>
-    <row r="79" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C79" s="11"/>
     </row>
-    <row r="80" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C80" s="11"/>
     </row>
-    <row r="81" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C81" s="11"/>
     </row>
-    <row r="82" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C82" s="11"/>
     </row>
-    <row r="83" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C83" s="11"/>
     </row>
-    <row r="84" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C84" s="11"/>
     </row>
-    <row r="85" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C85" s="11"/>
     </row>
-    <row r="86" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C86" s="11"/>
     </row>
-    <row r="87" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C87" s="11"/>
     </row>
-    <row r="88" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C88" s="11"/>
     </row>
-    <row r="89" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C89" s="11"/>
     </row>
-    <row r="90" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C90" s="11"/>
     </row>
-    <row r="91" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C91" s="11"/>
     </row>
-    <row r="92" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C92" s="11"/>
     </row>
-    <row r="93" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C93" s="11"/>
     </row>
-    <row r="94" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C94" s="11"/>
     </row>
-    <row r="95" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C95" s="11"/>
     </row>
-    <row r="96" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C96" s="11"/>
     </row>
-    <row r="97" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C97" s="11"/>
     </row>
-    <row r="98" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C98" s="11"/>
     </row>
-    <row r="99" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C99" s="11"/>
     </row>
-    <row r="100" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C100" s="11"/>
     </row>
-    <row r="101" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C101" s="11"/>
     </row>
-    <row r="102" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C102" s="11"/>
     </row>
-    <row r="103" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C103" s="11"/>
     </row>
-    <row r="104" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C104" s="11"/>
     </row>
-    <row r="105" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C105" s="11"/>
     </row>
-    <row r="106" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C106" s="11"/>
     </row>
-    <row r="107" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C107" s="11"/>
     </row>
-    <row r="108" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C108" s="11"/>
     </row>
-    <row r="109" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C109" s="11"/>
     </row>
-    <row r="110" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C110" s="11"/>
     </row>
-    <row r="111" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C111" s="11"/>
     </row>
-    <row r="112" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C112" s="11"/>
     </row>
-    <row r="113" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C113" s="11"/>
     </row>
-    <row r="114" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C114" s="11"/>
     </row>
-    <row r="115" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C115" s="11"/>
     </row>
-    <row r="116" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C116" s="11"/>
     </row>
-    <row r="117" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C117" s="11"/>
     </row>
-    <row r="118" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C118" s="11"/>
     </row>
-    <row r="119" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C119" s="11"/>
     </row>
-    <row r="120" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C120" s="11"/>
     </row>
-    <row r="121" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C121" s="11"/>
     </row>
-    <row r="122" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C122" s="11"/>
     </row>
-    <row r="123" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C123" s="11"/>
     </row>
-    <row r="124" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C124" s="11"/>
     </row>
-    <row r="125" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C125" s="11"/>
     </row>
-    <row r="126" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C126" s="11"/>
     </row>
-    <row r="127" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C127" s="11"/>
     </row>
-    <row r="128" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C128" s="11"/>
     </row>
-    <row r="129" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C129" s="11"/>
     </row>
-    <row r="130" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C130" s="11"/>
     </row>
-    <row r="131" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C131" s="11"/>
     </row>
-    <row r="132" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C132" s="11"/>
     </row>
-    <row r="133" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C133" s="11"/>
     </row>
-    <row r="134" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C134" s="11"/>
     </row>
-    <row r="135" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C135" s="11"/>
     </row>
-    <row r="136" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C136" s="11"/>
     </row>
-    <row r="137" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C137" s="11"/>
     </row>
-    <row r="138" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C138" s="11"/>
     </row>
-    <row r="139" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C139" s="11"/>
     </row>
-    <row r="140" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C140" s="11"/>
     </row>
-    <row r="141" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C141" s="11"/>
     </row>
-    <row r="142" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C142" s="11"/>
     </row>
-    <row r="143" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C143" s="11"/>
     </row>
-    <row r="144" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C144" s="11"/>
     </row>
-    <row r="145" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C145" s="11"/>
     </row>
-    <row r="146" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C146" s="11"/>
     </row>
-    <row r="147" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C147" s="11"/>
     </row>
-    <row r="148" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C148" s="11"/>
     </row>
-    <row r="149" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C149" s="11"/>
     </row>
-    <row r="150" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C150" s="11"/>
     </row>
-    <row r="151" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C151" s="11"/>
     </row>
-    <row r="152" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C152" s="11"/>
     </row>
-    <row r="153" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C153" s="11"/>
     </row>
-    <row r="154" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C154" s="11"/>
     </row>
-    <row r="155" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C155" s="11"/>
     </row>
-    <row r="156" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C156" s="11"/>
     </row>
-    <row r="157" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C157" s="11"/>
     </row>
-    <row r="158" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C158" s="11"/>
     </row>
-    <row r="159" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C159" s="11"/>
     </row>
-    <row r="160" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C160" s="11"/>
     </row>
-    <row r="161" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C161" s="11"/>
     </row>
-    <row r="162" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C162" s="11"/>
     </row>
-    <row r="163" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C163" s="11"/>
     </row>
-    <row r="164" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C164" s="11"/>
     </row>
-    <row r="165" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C165" s="11"/>
     </row>
-    <row r="166" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C166" s="11"/>
     </row>
-    <row r="167" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C167" s="11"/>
     </row>
-    <row r="168" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C168" s="11"/>
     </row>
-    <row r="169" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C169" s="11"/>
     </row>
-    <row r="170" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C170" s="11"/>
     </row>
-    <row r="171" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C171" s="11"/>
     </row>
-    <row r="172" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C172" s="11"/>
     </row>
-    <row r="173" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C173" s="11"/>
     </row>
-    <row r="174" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C174" s="11"/>
     </row>
-    <row r="175" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C175" s="11"/>
     </row>
-    <row r="176" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C176" s="11"/>
     </row>
-    <row r="177" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C177" s="11"/>
     </row>
-    <row r="178" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C178" s="11"/>
     </row>
-    <row r="179" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C179" s="11"/>
     </row>
-    <row r="180" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C180" s="11"/>
     </row>
-    <row r="181" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C181" s="11"/>
     </row>
-    <row r="182" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C182" s="11"/>
     </row>
-    <row r="183" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C183" s="11"/>
     </row>
-    <row r="184" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C184" s="11"/>
     </row>
-    <row r="185" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C185" s="11"/>
     </row>
-    <row r="186" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C186" s="11"/>
     </row>
-    <row r="187" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C187" s="11"/>
     </row>
-    <row r="188" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C188" s="11"/>
     </row>
-    <row r="189" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C189" s="11"/>
     </row>
-    <row r="190" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C190" s="11"/>
     </row>
-    <row r="191" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C191" s="11"/>
     </row>
-    <row r="192" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C192" s="11"/>
     </row>
-    <row r="193" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C193" s="11"/>
     </row>
-    <row r="194" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C194" s="11"/>
     </row>
-    <row r="195" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C195" s="11"/>
     </row>
-    <row r="196" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C196" s="11"/>
     </row>
-    <row r="197" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C197" s="11"/>
     </row>
-    <row r="198" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C198" s="11"/>
     </row>
-    <row r="199" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C199" s="11"/>
     </row>
-    <row r="200" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C200" s="11"/>
     </row>
-    <row r="201" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C201" s="11"/>
     </row>
-    <row r="202" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C202" s="11"/>
     </row>
-    <row r="203" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C203" s="11"/>
     </row>
-    <row r="204" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C204" s="11"/>
     </row>
-    <row r="205" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C205" s="11"/>
     </row>
-    <row r="206" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C206" s="11"/>
     </row>
-    <row r="207" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C207" s="11"/>
     </row>
-    <row r="208" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C208" s="11"/>
     </row>
-    <row r="209" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C209" s="11"/>
     </row>
-    <row r="210" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C210" s="11"/>
     </row>
-    <row r="211" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C211" s="11"/>
     </row>
-    <row r="212" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C212" s="11"/>
     </row>
-    <row r="213" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C213" s="11"/>
     </row>
-    <row r="214" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C214" s="11"/>
     </row>
-    <row r="215" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C215" s="11"/>
     </row>
-    <row r="216" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C216" s="11"/>
     </row>
-    <row r="217" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C217" s="11"/>
     </row>
-    <row r="218" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C218" s="11"/>
     </row>
-    <row r="219" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C219" s="11"/>
     </row>
-    <row r="220" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C220" s="11"/>
     </row>
-    <row r="221" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C221" s="11"/>
     </row>
-    <row r="222" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C222" s="11"/>
     </row>
-    <row r="223" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C223" s="11"/>
     </row>
-    <row r="224" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C224" s="11"/>
     </row>
-    <row r="225" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C225" s="11"/>
     </row>
-    <row r="226" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C226" s="11"/>
     </row>
-    <row r="227" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C227" s="11"/>
     </row>
-    <row r="228" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C228" s="11"/>
     </row>
-    <row r="229" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C229" s="11"/>
     </row>
-    <row r="230" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C230" s="11"/>
     </row>
-    <row r="231" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C231" s="11"/>
     </row>
-    <row r="232" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C232" s="11"/>
     </row>
-    <row r="233" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C233" s="11"/>
     </row>
-    <row r="234" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C234" s="11"/>
     </row>
-    <row r="235" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C235" s="11"/>
     </row>
-    <row r="236" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C236" s="11"/>
     </row>
-    <row r="237" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C237" s="11"/>
     </row>
-    <row r="238" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C238" s="11"/>
     </row>
-    <row r="239" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C239" s="11"/>
     </row>
-    <row r="240" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C240" s="11"/>
     </row>
-    <row r="241" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C241" s="11"/>
     </row>
-    <row r="242" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C242" s="11"/>
     </row>
-    <row r="243" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C243" s="11"/>
     </row>
-    <row r="244" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C244" s="11"/>
     </row>
-    <row r="245" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C245" s="11"/>
     </row>
-    <row r="246" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C246" s="11"/>
     </row>
-    <row r="247" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C247" s="11"/>
     </row>
-    <row r="248" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C248" s="11"/>
     </row>
-    <row r="249" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C249" s="11"/>
     </row>
-    <row r="250" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C250" s="11"/>
     </row>
-    <row r="251" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C251" s="11"/>
     </row>
-    <row r="252" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C252" s="11"/>
     </row>
-    <row r="253" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C253" s="11"/>
     </row>
-    <row r="254" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C254" s="11"/>
     </row>
-    <row r="255" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C255" s="11"/>
     </row>
-    <row r="256" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C256" s="11"/>
     </row>
-    <row r="257" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C257" s="11"/>
     </row>
-    <row r="258" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C258" s="11"/>
     </row>
-    <row r="259" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C259" s="11"/>
     </row>
-    <row r="260" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C260" s="11"/>
     </row>
-    <row r="261" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C261" s="11"/>
     </row>
-    <row r="262" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C262" s="11"/>
     </row>
-    <row r="263" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C263" s="11"/>
     </row>
-    <row r="264" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C264" s="11"/>
     </row>
-    <row r="265" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C265" s="11"/>
     </row>
-    <row r="266" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C266" s="11"/>
     </row>
-    <row r="267" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C267" s="11"/>
     </row>
-    <row r="268" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C268" s="11"/>
     </row>
-    <row r="269" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C269" s="11"/>
     </row>
-    <row r="270" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C270" s="11"/>
     </row>
-    <row r="271" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C271" s="11"/>
     </row>
-    <row r="272" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C272" s="11"/>
     </row>
-    <row r="273" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C273" s="11"/>
     </row>
-    <row r="274" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C274" s="11"/>
     </row>
-    <row r="275" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C275" s="11"/>
     </row>
-    <row r="276" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C276" s="11"/>
     </row>
-    <row r="277" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C277" s="11"/>
     </row>
-    <row r="278" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C278" s="11"/>
     </row>
-    <row r="279" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C279" s="11"/>
     </row>
-    <row r="280" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C280" s="11"/>
     </row>
-    <row r="281" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C281" s="11"/>
     </row>
-    <row r="282" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C282" s="11"/>
     </row>
-    <row r="283" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C283" s="11"/>
     </row>
-    <row r="284" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C284" s="11"/>
     </row>
-    <row r="285" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C285" s="11"/>
     </row>
-    <row r="286" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C286" s="11"/>
     </row>
-    <row r="287" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C287" s="11"/>
     </row>
-    <row r="288" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C288" s="11"/>
     </row>
-    <row r="289" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C289" s="11"/>
     </row>
-    <row r="290" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C290" s="11"/>
     </row>
-    <row r="291" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C291" s="11"/>
     </row>
-    <row r="292" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C292" s="11"/>
     </row>
-    <row r="293" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C293" s="11"/>
     </row>
-    <row r="294" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C294" s="11"/>
     </row>
-    <row r="295" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="295" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C295" s="11"/>
     </row>
-    <row r="296" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="296" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C296" s="11"/>
     </row>
-    <row r="297" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="297" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C297" s="11"/>
     </row>
-    <row r="298" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="298" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C298" s="11"/>
     </row>
-    <row r="299" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C299" s="11"/>
     </row>
-    <row r="300" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C300" s="11"/>
     </row>
-    <row r="301" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C301" s="11"/>
     </row>
-    <row r="302" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="302" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C302" s="11"/>
     </row>
-    <row r="303" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="303" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C303" s="11"/>
     </row>
-    <row r="304" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="304" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C304" s="11"/>
     </row>
-    <row r="305" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="305" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C305" s="11"/>
     </row>
-    <row r="306" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="306" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C306" s="11"/>
     </row>
-    <row r="307" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="307" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C307" s="11"/>
     </row>
-    <row r="308" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C308" s="11"/>
     </row>
-    <row r="309" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C309" s="11"/>
     </row>
-    <row r="310" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C310" s="11"/>
     </row>
-    <row r="311" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C311" s="11"/>
     </row>
-    <row r="312" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="312" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C312" s="11"/>
     </row>
-    <row r="313" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="313" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C313" s="11"/>
     </row>
-    <row r="314" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="314" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C314" s="11"/>
     </row>
-    <row r="315" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="315" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C315" s="11"/>
     </row>
-    <row r="316" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="316" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C316" s="11"/>
     </row>
-    <row r="317" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="317" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C317" s="11"/>
     </row>
-    <row r="318" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="318" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C318" s="11"/>
     </row>
-    <row r="319" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="319" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C319" s="11"/>
     </row>
-    <row r="320" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="320" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C320" s="11"/>
     </row>
-    <row r="321" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="321" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C321" s="11"/>
     </row>
-    <row r="322" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="322" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C322" s="11"/>
     </row>
-    <row r="323" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="323" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C323" s="11"/>
     </row>
-    <row r="324" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="324" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C324" s="11"/>
     </row>
-    <row r="325" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="325" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C325" s="11"/>
     </row>
-    <row r="326" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="326" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C326" s="11"/>
     </row>
-    <row r="327" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="327" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C327" s="11"/>
     </row>
-    <row r="328" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="328" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C328" s="11"/>
     </row>
-    <row r="329" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="329" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C329" s="11"/>
     </row>
-    <row r="330" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="330" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C330" s="11"/>
     </row>
-    <row r="331" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="331" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C331" s="11"/>
     </row>
-    <row r="332" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="332" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C332" s="11"/>
     </row>
-    <row r="333" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="333" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C333" s="11"/>
     </row>
-    <row r="334" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="334" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C334" s="11"/>
     </row>
-    <row r="335" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="335" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C335" s="11"/>
     </row>
-    <row r="336" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="336" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C336" s="11"/>
     </row>
-    <row r="337" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="337" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C337" s="11"/>
     </row>
-    <row r="338" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="338" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C338" s="11"/>
     </row>
-    <row r="339" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="339" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C339" s="11"/>
     </row>
-    <row r="340" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="340" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C340" s="11"/>
     </row>
-    <row r="341" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="341" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C341" s="11"/>
     </row>
-    <row r="342" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="342" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C342" s="11"/>
     </row>
-    <row r="343" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="343" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C343" s="11"/>
     </row>
-    <row r="344" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="344" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C344" s="11"/>
     </row>
-    <row r="345" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="345" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C345" s="11"/>
     </row>
-    <row r="346" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="346" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C346" s="11"/>
     </row>
-    <row r="347" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="347" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C347" s="11"/>
     </row>
-    <row r="348" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="348" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C348" s="11"/>
     </row>
-    <row r="349" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="349" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C349" s="11"/>
     </row>
-    <row r="350" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="350" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C350" s="11"/>
     </row>
-    <row r="351" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="351" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C351" s="11"/>
     </row>
-    <row r="352" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="352" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C352" s="11"/>
     </row>
-    <row r="353" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C353" s="11"/>
     </row>
-    <row r="354" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C354" s="11"/>
     </row>
-    <row r="355" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C355" s="11"/>
     </row>
-    <row r="356" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="356" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C356" s="11"/>
     </row>
-    <row r="357" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C357" s="11"/>
     </row>
-    <row r="358" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="358" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C358" s="11"/>
     </row>
-    <row r="359" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="359" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C359" s="11"/>
     </row>
-    <row r="360" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C360" s="11"/>
     </row>
-    <row r="361" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="361" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C361" s="11"/>
     </row>
-    <row r="362" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C362" s="11"/>
     </row>
-    <row r="363" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="363" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C363" s="11"/>
     </row>
-    <row r="364" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="364" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C364" s="11"/>
     </row>
-    <row r="365" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C365" s="11"/>
     </row>
-    <row r="366" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="366" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C366" s="11"/>
     </row>
-    <row r="367" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="367" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C367" s="11"/>
     </row>
-    <row r="368" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="368" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C368" s="11"/>
     </row>
-    <row r="369" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C369" s="11"/>
     </row>
-    <row r="370" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C370" s="11"/>
     </row>
-    <row r="371" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C371" s="11"/>
     </row>
-    <row r="372" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="372" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C372" s="11"/>
     </row>
-    <row r="373" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="373" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C373" s="11"/>
     </row>
-    <row r="374" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="374" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C374" s="11"/>
     </row>
-    <row r="375" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="375" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C375" s="11"/>
     </row>
-    <row r="376" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="376" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C376" s="11"/>
     </row>
-    <row r="377" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="377" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C377" s="11"/>
     </row>
-    <row r="378" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="378" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C378" s="11"/>
     </row>
-    <row r="379" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="379" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C379" s="11"/>
     </row>
-    <row r="380" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="380" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C380" s="11"/>
     </row>
-    <row r="381" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="381" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C381" s="11"/>
     </row>
-    <row r="382" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="382" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C382" s="11"/>
     </row>
-    <row r="383" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="383" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C383" s="11"/>
     </row>
-    <row r="384" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="384" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C384" s="11"/>
     </row>
-    <row r="385" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="385" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C385" s="11"/>
     </row>
-    <row r="386" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="386" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C386" s="11"/>
     </row>
-    <row r="387" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="387" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C387" s="11"/>
     </row>
-    <row r="388" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="388" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C388" s="11"/>
     </row>
-    <row r="389" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="389" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C389" s="11"/>
     </row>
-    <row r="390" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="390" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C390" s="11"/>
     </row>
-    <row r="391" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="391" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C391" s="11"/>
     </row>
-    <row r="392" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="392" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C392" s="11"/>
     </row>
-    <row r="393" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="393" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C393" s="11"/>
     </row>
-    <row r="394" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="394" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C394" s="11"/>
     </row>
-    <row r="395" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="395" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C395" s="11"/>
     </row>
-    <row r="396" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="396" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C396" s="11"/>
     </row>
-    <row r="397" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="397" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C397" s="11"/>
     </row>
-    <row r="398" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="398" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C398" s="11"/>
     </row>
-    <row r="399" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="399" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C399" s="11"/>
     </row>
-    <row r="400" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="400" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C400" s="11"/>
     </row>
-    <row r="401" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="401" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C401" s="11"/>
     </row>
-    <row r="402" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="402" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C402" s="11"/>
     </row>
-    <row r="403" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="403" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C403" s="11"/>
     </row>
-    <row r="404" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="404" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C404" s="11"/>
     </row>
-    <row r="405" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="405" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C405" s="11"/>
     </row>
-    <row r="406" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="406" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C406" s="11"/>
     </row>
-    <row r="407" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="407" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C407" s="11"/>
     </row>
-    <row r="408" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="408" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C408" s="11"/>
     </row>
-    <row r="409" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="409" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C409" s="11"/>
     </row>
-    <row r="410" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="410" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C410" s="11"/>
     </row>
-    <row r="411" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="411" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C411" s="11"/>
     </row>
-    <row r="412" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="412" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C412" s="11"/>
     </row>
-    <row r="413" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="413" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C413" s="11"/>
     </row>
-    <row r="414" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="414" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C414" s="11"/>
     </row>
-    <row r="415" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="415" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C415" s="11"/>
     </row>
-    <row r="416" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="416" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C416" s="11"/>
     </row>
-    <row r="417" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="417" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C417" s="11"/>
     </row>
-    <row r="418" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="418" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C418" s="11"/>
     </row>
-    <row r="419" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="419" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C419" s="11"/>
     </row>
-    <row r="420" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="420" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C420" s="11"/>
     </row>
-    <row r="421" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="421" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C421" s="11"/>
     </row>
-    <row r="422" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="422" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C422" s="11"/>
     </row>
-    <row r="423" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="423" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C423" s="11"/>
     </row>
-    <row r="424" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="424" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C424" s="11"/>
     </row>
-    <row r="425" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="425" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C425" s="11"/>
     </row>
-    <row r="426" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="426" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C426" s="11"/>
     </row>
-    <row r="427" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="427" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C427" s="11"/>
     </row>
-    <row r="428" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="428" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C428" s="11"/>
     </row>
-    <row r="429" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="429" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C429" s="11"/>
     </row>
-    <row r="430" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="430" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C430" s="11"/>
     </row>
-    <row r="431" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="431" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C431" s="11"/>
     </row>
-    <row r="432" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="432" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C432" s="11"/>
     </row>
-    <row r="433" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="433" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C433" s="11"/>
     </row>
-    <row r="434" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="434" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C434" s="11"/>
     </row>
-    <row r="435" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="435" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C435" s="11"/>
     </row>
-    <row r="436" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="436" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C436" s="11"/>
     </row>
-    <row r="437" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="437" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C437" s="11"/>
     </row>
-    <row r="438" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="438" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C438" s="11"/>
     </row>
-    <row r="439" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="439" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C439" s="11"/>
     </row>
-    <row r="440" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="440" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C440" s="11"/>
     </row>
-    <row r="441" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="441" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C441" s="11"/>
     </row>
-    <row r="442" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="442" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C442" s="11"/>
     </row>
-    <row r="443" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="443" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C443" s="11"/>
     </row>
-    <row r="444" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="444" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C444" s="11"/>
     </row>
-    <row r="445" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="445" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C445" s="11"/>
     </row>
-    <row r="446" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="446" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C446" s="11"/>
     </row>
-    <row r="447" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="447" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C447" s="11"/>
     </row>
-    <row r="448" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="448" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C448" s="11"/>
     </row>
-    <row r="449" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="449" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C449" s="11"/>
     </row>
-    <row r="450" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="450" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C450" s="11"/>
     </row>
-    <row r="451" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="451" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C451" s="11"/>
     </row>
-    <row r="452" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="452" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C452" s="11"/>
     </row>
-    <row r="453" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="453" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C453" s="11"/>
     </row>
-    <row r="454" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="454" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C454" s="11"/>
     </row>
-    <row r="455" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="455" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C455" s="11"/>
     </row>
-    <row r="456" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="456" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C456" s="11"/>
     </row>
-    <row r="457" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="457" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C457" s="11"/>
     </row>
-    <row r="458" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="458" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C458" s="11"/>
     </row>
-    <row r="459" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="459" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C459" s="11"/>
     </row>
-    <row r="460" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="460" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C460" s="11"/>
     </row>
-    <row r="461" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="461" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C461" s="11"/>
     </row>
-    <row r="462" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="462" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C462" s="11"/>
     </row>
-    <row r="463" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="463" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C463" s="11"/>
     </row>
-    <row r="464" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="464" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C464" s="11"/>
     </row>
-    <row r="465" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="465" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C465" s="11"/>
     </row>
-    <row r="466" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="466" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C466" s="11"/>
     </row>
-    <row r="467" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="467" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C467" s="11"/>
     </row>
-    <row r="468" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="468" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C468" s="11"/>
     </row>
-    <row r="469" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="469" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C469" s="11"/>
     </row>
-    <row r="470" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="470" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C470" s="11"/>
     </row>
-    <row r="471" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="471" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C471" s="11"/>
     </row>
-    <row r="472" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="472" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C472" s="11"/>
     </row>
-    <row r="473" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="473" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C473" s="11"/>
     </row>
-    <row r="474" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="474" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C474" s="11"/>
     </row>
-    <row r="475" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="475" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C475" s="11"/>
     </row>
-    <row r="476" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="476" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C476" s="11"/>
     </row>
-    <row r="477" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="477" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C477" s="11"/>
     </row>
-    <row r="478" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="478" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C478" s="11"/>
     </row>
-    <row r="479" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="479" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C479" s="11"/>
     </row>
-    <row r="480" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="480" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C480" s="11"/>
     </row>
-    <row r="481" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="481" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C481" s="11"/>
     </row>
-    <row r="482" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="482" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C482" s="11"/>
     </row>
-    <row r="483" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="483" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C483" s="11"/>
     </row>
-    <row r="484" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="484" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C484" s="11"/>
     </row>
-    <row r="485" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="485" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C485" s="11"/>
     </row>
-    <row r="486" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="486" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C486" s="11"/>
     </row>
-    <row r="487" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="487" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C487" s="11"/>
     </row>
-    <row r="488" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="488" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C488" s="11"/>
     </row>
-    <row r="489" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="489" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C489" s="11"/>
     </row>
-    <row r="490" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="490" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C490" s="11"/>
     </row>
-    <row r="491" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="491" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C491" s="11"/>
     </row>
-    <row r="492" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="492" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C492" s="11"/>
     </row>
-    <row r="493" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="493" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C493" s="11"/>
     </row>
-    <row r="494" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="494" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C494" s="11"/>
     </row>
-    <row r="495" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="495" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C495" s="11"/>
     </row>
-    <row r="496" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="496" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C496" s="11"/>
     </row>
-    <row r="497" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="497" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C497" s="11"/>
     </row>
-    <row r="498" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="498" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C498" s="11"/>
     </row>
-    <row r="499" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="499" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C499" s="11"/>
     </row>
-    <row r="500" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="500" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C500" s="11"/>
     </row>
-    <row r="501" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="501" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C501" s="11"/>
     </row>
-    <row r="502" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="502" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C502" s="11"/>
     </row>
-    <row r="503" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="503" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C503" s="11"/>
     </row>
-    <row r="504" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="504" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C504" s="11"/>
     </row>
-    <row r="505" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="505" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C505" s="11"/>
     </row>
-    <row r="506" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="506" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C506" s="11"/>
     </row>
-    <row r="507" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="507" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C507" s="11"/>
     </row>
-    <row r="508" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="508" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C508" s="11"/>
     </row>
-    <row r="509" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="509" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C509" s="11"/>
     </row>
-    <row r="510" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="510" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C510" s="11"/>
     </row>
-    <row r="511" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="511" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C511" s="11"/>
     </row>
-    <row r="512" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="512" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C512" s="11"/>
     </row>
-    <row r="513" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="513" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C513" s="11"/>
     </row>
-    <row r="514" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="514" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C514" s="11"/>
     </row>
-    <row r="515" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="515" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C515" s="11"/>
     </row>
-    <row r="516" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="516" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C516" s="11"/>
     </row>
-    <row r="517" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="517" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C517" s="11"/>
     </row>
-    <row r="518" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="518" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C518" s="11"/>
     </row>
-    <row r="519" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="519" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C519" s="11"/>
     </row>
-    <row r="520" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="520" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C520" s="11"/>
     </row>
-    <row r="521" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="521" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C521" s="11"/>
     </row>
-    <row r="522" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="522" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C522" s="11"/>
     </row>
-    <row r="523" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="523" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C523" s="11"/>
     </row>
-    <row r="524" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="524" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C524" s="11"/>
     </row>
-    <row r="525" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="525" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C525" s="11"/>
     </row>
-    <row r="526" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="526" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C526" s="11"/>
     </row>
-    <row r="527" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="527" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C527" s="11"/>
     </row>
-    <row r="528" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="528" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C528" s="11"/>
     </row>
-    <row r="529" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="529" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C529" s="11"/>
     </row>
-    <row r="530" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="530" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C530" s="11"/>
     </row>
-    <row r="531" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="531" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C531" s="11"/>
     </row>
-    <row r="532" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="532" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C532" s="11"/>
     </row>
-    <row r="533" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="533" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C533" s="11"/>
     </row>
-    <row r="534" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="534" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C534" s="11"/>
     </row>
-    <row r="535" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="535" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C535" s="11"/>
     </row>
-    <row r="536" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="536" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C536" s="11"/>
     </row>
-    <row r="537" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="537" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C537" s="11"/>
     </row>
-    <row r="538" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="538" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C538" s="11"/>
     </row>
-    <row r="539" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="539" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C539" s="11"/>
     </row>
-    <row r="540" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="540" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C540" s="11"/>
     </row>
-    <row r="541" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="541" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C541" s="11"/>
     </row>
-    <row r="542" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="542" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C542" s="11"/>
     </row>
-    <row r="543" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="543" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C543" s="11"/>
     </row>
-    <row r="544" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="544" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C544" s="11"/>
     </row>
-    <row r="545" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="545" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C545" s="11"/>
     </row>
-    <row r="546" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="546" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C546" s="11"/>
     </row>
-    <row r="547" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="547" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C547" s="11"/>
     </row>
-    <row r="548" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="548" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C548" s="11"/>
     </row>
-    <row r="549" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="549" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C549" s="11"/>
     </row>
-    <row r="550" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="550" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C550" s="11"/>
     </row>
-    <row r="551" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="551" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C551" s="11"/>
     </row>
-    <row r="552" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="552" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C552" s="11"/>
     </row>
-    <row r="553" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="553" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C553" s="11"/>
     </row>
-    <row r="554" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="554" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C554" s="11"/>
     </row>
-    <row r="555" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="555" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C555" s="11"/>
     </row>
-    <row r="556" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="556" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C556" s="11"/>
     </row>
-    <row r="557" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="557" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C557" s="11"/>
     </row>
-    <row r="558" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="558" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C558" s="11"/>
     </row>
-    <row r="559" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="559" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C559" s="11"/>
     </row>
-    <row r="560" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="560" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C560" s="11"/>
     </row>
-    <row r="561" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="561" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C561" s="11"/>
     </row>
-    <row r="562" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="562" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C562" s="11"/>
     </row>
-    <row r="563" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="563" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C563" s="11"/>
     </row>
-    <row r="564" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="564" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C564" s="11"/>
     </row>
-    <row r="565" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="565" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C565" s="11"/>
     </row>
-    <row r="566" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="566" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C566" s="11"/>
     </row>
-    <row r="567" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="567" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C567" s="11"/>
     </row>
-    <row r="568" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="568" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C568" s="11"/>
     </row>
-    <row r="569" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="569" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C569" s="11"/>
     </row>
-    <row r="570" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="570" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C570" s="11"/>
     </row>
-    <row r="571" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="571" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C571" s="11"/>
     </row>
-    <row r="572" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="572" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C572" s="11"/>
     </row>
-    <row r="573" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="573" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C573" s="11"/>
     </row>
-    <row r="574" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="574" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C574" s="11"/>
     </row>
-    <row r="575" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="575" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C575" s="11"/>
     </row>
-    <row r="576" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="576" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C576" s="11"/>
     </row>
-    <row r="577" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="577" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C577" s="11"/>
     </row>
-    <row r="578" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="578" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C578" s="11"/>
     </row>
-    <row r="579" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="579" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C579" s="11"/>
     </row>
-    <row r="580" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="580" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C580" s="11"/>
     </row>
-    <row r="581" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="581" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C581" s="11"/>
     </row>
-    <row r="582" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="582" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C582" s="11"/>
     </row>
-    <row r="583" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="583" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C583" s="11"/>
     </row>
-    <row r="584" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="584" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C584" s="11"/>
     </row>
-    <row r="585" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="585" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C585" s="11"/>
     </row>
-    <row r="586" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="586" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C586" s="11"/>
     </row>
-    <row r="587" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="587" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C587" s="11"/>
     </row>
-    <row r="588" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="588" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C588" s="11"/>
     </row>
-    <row r="589" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="589" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C589" s="11"/>
     </row>
-    <row r="590" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="590" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C590" s="11"/>
     </row>
-    <row r="591" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="591" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C591" s="11"/>
     </row>
-    <row r="592" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="592" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C592" s="11"/>
     </row>
-    <row r="593" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="593" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C593" s="11"/>
     </row>
-    <row r="594" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="594" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C594" s="11"/>
     </row>
-    <row r="595" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="595" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C595" s="11"/>
     </row>
-    <row r="596" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="596" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C596" s="11"/>
     </row>
-    <row r="597" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="597" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C597" s="11"/>
     </row>
-    <row r="598" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="598" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C598" s="11"/>
     </row>
-    <row r="599" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="599" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C599" s="11"/>
     </row>
-    <row r="600" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="600" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C600" s="11"/>
     </row>
-    <row r="601" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="601" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C601" s="11"/>
     </row>
-    <row r="602" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="602" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C602" s="11"/>
     </row>
-    <row r="603" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="603" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C603" s="11"/>
     </row>
-    <row r="604" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="604" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C604" s="11"/>
     </row>
-    <row r="605" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="605" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C605" s="11"/>
     </row>
-    <row r="606" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="606" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C606" s="11"/>
     </row>
-    <row r="607" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="607" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C607" s="11"/>
     </row>
-    <row r="608" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="608" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C608" s="11"/>
     </row>
-    <row r="609" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="609" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C609" s="11"/>
     </row>
-    <row r="610" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="610" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C610" s="11"/>
     </row>
-    <row r="611" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="611" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C611" s="11"/>
     </row>
-    <row r="612" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="612" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C612" s="11"/>
     </row>
-    <row r="613" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="613" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C613" s="11"/>
     </row>
-    <row r="614" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="614" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C614" s="11"/>
     </row>
-    <row r="615" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="615" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C615" s="11"/>
     </row>
-    <row r="616" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="616" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C616" s="11"/>
     </row>
-    <row r="617" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="617" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C617" s="11"/>
     </row>
-    <row r="618" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="618" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C618" s="11"/>
     </row>
-    <row r="619" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="619" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C619" s="11"/>
     </row>
-    <row r="620" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="620" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C620" s="11"/>
     </row>
-    <row r="621" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="621" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C621" s="11"/>
     </row>
-    <row r="622" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="622" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C622" s="11"/>
     </row>
-    <row r="623" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="623" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C623" s="11"/>
     </row>
-    <row r="624" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="624" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C624" s="11"/>
     </row>
-    <row r="625" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="625" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C625" s="11"/>
     </row>
-    <row r="626" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="626" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C626" s="11"/>
     </row>
-    <row r="627" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="627" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C627" s="11"/>
     </row>
-    <row r="628" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="628" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C628" s="11"/>
     </row>
-    <row r="629" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="629" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C629" s="11"/>
     </row>
-    <row r="630" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="630" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C630" s="11"/>
     </row>
-    <row r="631" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="631" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C631" s="11"/>
     </row>
-    <row r="632" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="632" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C632" s="11"/>
     </row>
-    <row r="633" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="633" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C633" s="11"/>
     </row>
-    <row r="634" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="634" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C634" s="11"/>
     </row>
-    <row r="635" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="635" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C635" s="11"/>
     </row>
-    <row r="636" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="636" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C636" s="11"/>
     </row>
-    <row r="637" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="637" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C637" s="11"/>
     </row>
-    <row r="638" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="638" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C638" s="11"/>
     </row>
-    <row r="639" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="639" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C639" s="11"/>
     </row>
-    <row r="640" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="640" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C640" s="11"/>
     </row>
-    <row r="641" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="641" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C641" s="11"/>
     </row>
-    <row r="642" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="642" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C642" s="11"/>
     </row>
-    <row r="643" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="643" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C643" s="11"/>
     </row>
-    <row r="644" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="644" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C644" s="11"/>
     </row>
-    <row r="645" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="645" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C645" s="11"/>
     </row>
-    <row r="646" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="646" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C646" s="11"/>
     </row>
-    <row r="647" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="647" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C647" s="11"/>
     </row>
-    <row r="648" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="648" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C648" s="11"/>
     </row>
-    <row r="649" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="649" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C649" s="11"/>
     </row>
-    <row r="650" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="650" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C650" s="11"/>
     </row>
-    <row r="651" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="651" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C651" s="11"/>
     </row>
-    <row r="652" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="652" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C652" s="11"/>
     </row>
-    <row r="653" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="653" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C653" s="11"/>
     </row>
-    <row r="654" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="654" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C654" s="11"/>
     </row>
-    <row r="655" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="655" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C655" s="11"/>
     </row>
-    <row r="656" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="656" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C656" s="11"/>
     </row>
-    <row r="657" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="657" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C657" s="11"/>
     </row>
-    <row r="658" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="658" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C658" s="11"/>
     </row>
-    <row r="659" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="659" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C659" s="11"/>
     </row>
-    <row r="660" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="660" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C660" s="11"/>
     </row>
-    <row r="661" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="661" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C661" s="11"/>
     </row>
-    <row r="662" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="662" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C662" s="11"/>
     </row>
-    <row r="663" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="663" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C663" s="11"/>
     </row>
-    <row r="664" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="664" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C664" s="11"/>
     </row>
-    <row r="665" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="665" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C665" s="11"/>
     </row>
-    <row r="666" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="666" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C666" s="11"/>
     </row>
-    <row r="667" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="667" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C667" s="11"/>
     </row>
-    <row r="668" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="668" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C668" s="11"/>
     </row>
-    <row r="669" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="669" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C669" s="11"/>
     </row>
-    <row r="670" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="670" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C670" s="11"/>
     </row>
-    <row r="671" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="671" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C671" s="11"/>
     </row>
-    <row r="672" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="672" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C672" s="11"/>
     </row>
-    <row r="673" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="673" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C673" s="11"/>
     </row>
-    <row r="674" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="674" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C674" s="11"/>
     </row>
-    <row r="675" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="675" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C675" s="11"/>
     </row>
-    <row r="676" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="676" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C676" s="11"/>
     </row>
-    <row r="677" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="677" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C677" s="11"/>
     </row>
-    <row r="678" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="678" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C678" s="11"/>
     </row>
-    <row r="679" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="679" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C679" s="11"/>
     </row>
-    <row r="680" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="680" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C680" s="11"/>
     </row>
-    <row r="681" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="681" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C681" s="11"/>
     </row>
-    <row r="682" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="682" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C682" s="11"/>
     </row>
-    <row r="683" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="683" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C683" s="11"/>
     </row>
-    <row r="684" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="684" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C684" s="11"/>
     </row>
-    <row r="685" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="685" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C685" s="11"/>
     </row>
-    <row r="686" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="686" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C686" s="11"/>
     </row>
-    <row r="687" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="687" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C687" s="11"/>
     </row>
-    <row r="688" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="688" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C688" s="11"/>
     </row>
-    <row r="689" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="689" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C689" s="11"/>
     </row>
-    <row r="690" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="690" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C690" s="11"/>
     </row>
-    <row r="691" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="691" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C691" s="11"/>
     </row>
-    <row r="692" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="692" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C692" s="11"/>
     </row>
-    <row r="693" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="693" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C693" s="11"/>
     </row>
-    <row r="694" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="694" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C694" s="11"/>
     </row>
-    <row r="695" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="695" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C695" s="11"/>
     </row>
-    <row r="696" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="696" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C696" s="11"/>
     </row>
-    <row r="697" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="697" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C697" s="11"/>
     </row>
-    <row r="698" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="698" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C698" s="11"/>
     </row>
-    <row r="699" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="699" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C699" s="11"/>
     </row>
-    <row r="700" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="700" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C700" s="11"/>
     </row>
-    <row r="701" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="701" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C701" s="11"/>
     </row>
-    <row r="702" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="702" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C702" s="11"/>
     </row>
-    <row r="703" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="703" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C703" s="11"/>
     </row>
-    <row r="704" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="704" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C704" s="11"/>
     </row>
-    <row r="705" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="705" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C705" s="11"/>
     </row>
-    <row r="706" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="706" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C706" s="11"/>
     </row>
-    <row r="707" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="707" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C707" s="11"/>
     </row>
-    <row r="708" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="708" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C708" s="11"/>
     </row>
-    <row r="709" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="709" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C709" s="11"/>
     </row>
-    <row r="710" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="710" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C710" s="11"/>
     </row>
-    <row r="711" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="711" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C711" s="11"/>
     </row>
-    <row r="712" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="712" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C712" s="11"/>
     </row>
-    <row r="713" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="713" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C713" s="11"/>
     </row>
-    <row r="714" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="714" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C714" s="11"/>
     </row>
-    <row r="715" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="715" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C715" s="11"/>
     </row>
-    <row r="716" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="716" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C716" s="11"/>
     </row>
-    <row r="717" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="717" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C717" s="11"/>
     </row>
-    <row r="718" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="718" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C718" s="11"/>
     </row>
-    <row r="719" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="719" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C719" s="11"/>
     </row>
-    <row r="720" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="720" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C720" s="11"/>
     </row>
-    <row r="721" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="721" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C721" s="11"/>
     </row>
-    <row r="722" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="722" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C722" s="11"/>
     </row>
-    <row r="723" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="723" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C723" s="11"/>
     </row>
-    <row r="724" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="724" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C724" s="11"/>
     </row>
-    <row r="725" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="725" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C725" s="11"/>
     </row>
-    <row r="726" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="726" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C726" s="11"/>
     </row>
-    <row r="727" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="727" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C727" s="11"/>
     </row>
-    <row r="728" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="728" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C728" s="11"/>
     </row>
-    <row r="729" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="729" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C729" s="11"/>
     </row>
-    <row r="730" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="730" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C730" s="11"/>
     </row>
-    <row r="731" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="731" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C731" s="11"/>
     </row>
-    <row r="732" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="732" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C732" s="11"/>
     </row>
-    <row r="733" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="733" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C733" s="11"/>
     </row>
-    <row r="734" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="734" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C734" s="11"/>
     </row>
-    <row r="735" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="735" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C735" s="11"/>
     </row>
-    <row r="736" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="736" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C736" s="11"/>
     </row>
-    <row r="737" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="737" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C737" s="11"/>
     </row>
-    <row r="738" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="738" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C738" s="11"/>
     </row>
-    <row r="739" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="739" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C739" s="11"/>
     </row>
-    <row r="740" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="740" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C740" s="11"/>
     </row>
-    <row r="741" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="741" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C741" s="11"/>
     </row>
-    <row r="742" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="742" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C742" s="11"/>
     </row>
-    <row r="743" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="743" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C743" s="11"/>
     </row>
-    <row r="744" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="744" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C744" s="11"/>
     </row>
-    <row r="745" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="745" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C745" s="11"/>
     </row>
-    <row r="746" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="746" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C746" s="11"/>
     </row>
-    <row r="747" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="747" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C747" s="11"/>
     </row>
-    <row r="748" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="748" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C748" s="11"/>
     </row>
-    <row r="749" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="749" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C749" s="11"/>
     </row>
-    <row r="750" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="750" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C750" s="11"/>
     </row>
-    <row r="751" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="751" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C751" s="11"/>
     </row>
-    <row r="752" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="752" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C752" s="11"/>
     </row>
-    <row r="753" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="753" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C753" s="11"/>
     </row>
-    <row r="754" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="754" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C754" s="11"/>
     </row>
-    <row r="755" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="755" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C755" s="11"/>
     </row>
-    <row r="756" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="756" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C756" s="11"/>
     </row>
-    <row r="757" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="757" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C757" s="11"/>
     </row>
-    <row r="758" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="758" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C758" s="11"/>
     </row>
-    <row r="759" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="759" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C759" s="11"/>
     </row>
-    <row r="760" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="760" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C760" s="11"/>
     </row>
-    <row r="761" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="761" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C761" s="11"/>
     </row>
-    <row r="762" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="762" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C762" s="11"/>
     </row>
-    <row r="763" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="763" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C763" s="11"/>
     </row>
-    <row r="764" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="764" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C764" s="11"/>
     </row>
-    <row r="765" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="765" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C765" s="11"/>
     </row>
-    <row r="766" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="766" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C766" s="11"/>
     </row>
-    <row r="767" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="767" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C767" s="11"/>
     </row>
-    <row r="768" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="768" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C768" s="11"/>
     </row>
-    <row r="769" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="769" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C769" s="11"/>
     </row>
-    <row r="770" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="770" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C770" s="11"/>
     </row>
-    <row r="771" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="771" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C771" s="11"/>
     </row>
-    <row r="772" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="772" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C772" s="11"/>
     </row>
-    <row r="773" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="773" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C773" s="11"/>
     </row>
-    <row r="774" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="774" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C774" s="11"/>
     </row>
-    <row r="775" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="775" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C775" s="11"/>
     </row>
-    <row r="776" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="776" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C776" s="11"/>
     </row>
-    <row r="777" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="777" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C777" s="11"/>
     </row>
-    <row r="778" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="778" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C778" s="11"/>
     </row>
-    <row r="779" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="779" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C779" s="11"/>
     </row>
-    <row r="780" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="780" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C780" s="11"/>
     </row>
-    <row r="781" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="781" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C781" s="11"/>
     </row>
-    <row r="782" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="782" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C782" s="11"/>
     </row>
-    <row r="783" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="783" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C783" s="11"/>
     </row>
-    <row r="784" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="784" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C784" s="11"/>
     </row>
-    <row r="785" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="785" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C785" s="11"/>
     </row>
-    <row r="786" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="786" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C786" s="11"/>
     </row>
-    <row r="787" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="787" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C787" s="11"/>
     </row>
-    <row r="788" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="788" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C788" s="11"/>
     </row>
-    <row r="789" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="789" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C789" s="11"/>
     </row>
-    <row r="790" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="790" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C790" s="11"/>
     </row>
-    <row r="791" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="791" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C791" s="11"/>
     </row>
-    <row r="792" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="792" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C792" s="11"/>
     </row>
-    <row r="793" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="793" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C793" s="11"/>
     </row>
-    <row r="794" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="794" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C794" s="11"/>
     </row>
-    <row r="795" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="795" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C795" s="11"/>
     </row>
-    <row r="796" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="796" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C796" s="11"/>
     </row>
-    <row r="797" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="797" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C797" s="11"/>
     </row>
-    <row r="798" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="798" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C798" s="11"/>
     </row>
-    <row r="799" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="799" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C799" s="11"/>
     </row>
-    <row r="800" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="800" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C800" s="11"/>
     </row>
-    <row r="801" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="801" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C801" s="11"/>
     </row>
-    <row r="802" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="802" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C802" s="11"/>
     </row>
-    <row r="803" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="803" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C803" s="11"/>
     </row>
-    <row r="804" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="804" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C804" s="11"/>
     </row>
-    <row r="805" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="805" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C805" s="11"/>
     </row>
-    <row r="806" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="806" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C806" s="11"/>
     </row>
-    <row r="807" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="807" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C807" s="11"/>
     </row>
-    <row r="808" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="808" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C808" s="11"/>
     </row>
-    <row r="809" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="809" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C809" s="11"/>
     </row>
-    <row r="810" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="810" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C810" s="11"/>
     </row>
-    <row r="811" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="811" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C811" s="11"/>
     </row>
-    <row r="812" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="812" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C812" s="11"/>
     </row>
-    <row r="813" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="813" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C813" s="11"/>
     </row>
-    <row r="814" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="814" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C814" s="11"/>
     </row>
-    <row r="815" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="815" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C815" s="11"/>
     </row>
-    <row r="816" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="816" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C816" s="11"/>
     </row>
-    <row r="817" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="817" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C817" s="11"/>
     </row>
-    <row r="818" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="818" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C818" s="11"/>
     </row>
-    <row r="819" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="819" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C819" s="11"/>
     </row>
-    <row r="820" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="820" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C820" s="11"/>
     </row>
-    <row r="821" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="821" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C821" s="11"/>
     </row>
-    <row r="822" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="822" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C822" s="11"/>
     </row>
-    <row r="823" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="823" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C823" s="11"/>
     </row>
-    <row r="824" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="824" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C824" s="11"/>
     </row>
-    <row r="825" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="825" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C825" s="11"/>
     </row>
-    <row r="826" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="826" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C826" s="11"/>
     </row>
-    <row r="827" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="827" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C827" s="11"/>
     </row>
-    <row r="828" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="828" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C828" s="11"/>
     </row>
-    <row r="829" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="829" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C829" s="11"/>
     </row>
-    <row r="830" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="830" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C830" s="11"/>
     </row>
-    <row r="831" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="831" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C831" s="11"/>
     </row>
-    <row r="832" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="832" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C832" s="11"/>
     </row>
-    <row r="833" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="833" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C833" s="11"/>
     </row>
-    <row r="834" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="834" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C834" s="11"/>
     </row>
-    <row r="835" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="835" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C835" s="11"/>
     </row>
-    <row r="836" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="836" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C836" s="11"/>
     </row>
-    <row r="837" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="837" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C837" s="11"/>
     </row>
-    <row r="838" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="838" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C838" s="11"/>
     </row>
-    <row r="839" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="839" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C839" s="11"/>
     </row>
-    <row r="840" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="840" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C840" s="11"/>
     </row>
-    <row r="841" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="841" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C841" s="11"/>
     </row>
-    <row r="842" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="842" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C842" s="11"/>
     </row>
-    <row r="843" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="843" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C843" s="11"/>
     </row>
-    <row r="844" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="844" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C844" s="11"/>
     </row>
-    <row r="845" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="845" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C845" s="11"/>
     </row>
-    <row r="846" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="846" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C846" s="11"/>
     </row>
-    <row r="847" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="847" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C847" s="11"/>
     </row>
-    <row r="848" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="848" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C848" s="11"/>
     </row>
-    <row r="849" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="849" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C849" s="11"/>
     </row>
-    <row r="850" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="850" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C850" s="11"/>
     </row>
-    <row r="851" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="851" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C851" s="11"/>
     </row>
-    <row r="852" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="852" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C852" s="11"/>
     </row>
-    <row r="853" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="853" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C853" s="11"/>
     </row>
-    <row r="854" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="854" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C854" s="11"/>
     </row>
-    <row r="855" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="855" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C855" s="11"/>
     </row>
-    <row r="856" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="856" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C856" s="11"/>
     </row>
-    <row r="857" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="857" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C857" s="11"/>
     </row>
-    <row r="858" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="858" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C858" s="11"/>
     </row>
-    <row r="859" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="859" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C859" s="11"/>
     </row>
-    <row r="860" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="860" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C860" s="11"/>
     </row>
-    <row r="861" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="861" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C861" s="11"/>
     </row>
-    <row r="862" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="862" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C862" s="11"/>
     </row>
-    <row r="863" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="863" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C863" s="11"/>
     </row>
-    <row r="864" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="864" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C864" s="11"/>
     </row>
-    <row r="865" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="865" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C865" s="11"/>
     </row>
-    <row r="866" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="866" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C866" s="11"/>
     </row>
-    <row r="867" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="867" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C867" s="11"/>
     </row>
-    <row r="868" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="868" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C868" s="11"/>
     </row>
-    <row r="869" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="869" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C869" s="11"/>
     </row>
-    <row r="870" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="870" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C870" s="11"/>
     </row>
-    <row r="871" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="871" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C871" s="11"/>
     </row>
-    <row r="872" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="872" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C872" s="11"/>
     </row>
-    <row r="873" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="873" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C873" s="11"/>
     </row>
-    <row r="874" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="874" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C874" s="11"/>
     </row>
-    <row r="875" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="875" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C875" s="11"/>
     </row>
-    <row r="876" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="876" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C876" s="11"/>
     </row>
-    <row r="877" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="877" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C877" s="11"/>
     </row>
-    <row r="878" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="878" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C878" s="11"/>
     </row>
-    <row r="879" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="879" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C879" s="11"/>
     </row>
-    <row r="880" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="880" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C880" s="11"/>
     </row>
-    <row r="881" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="881" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C881" s="11"/>
     </row>
-    <row r="882" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="882" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C882" s="11"/>
     </row>
-    <row r="883" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="883" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C883" s="11"/>
     </row>
-    <row r="884" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="884" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C884" s="11"/>
     </row>
-    <row r="885" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="885" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C885" s="11"/>
     </row>
-    <row r="886" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="886" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C886" s="11"/>
     </row>
-    <row r="887" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="887" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C887" s="11"/>
     </row>
-    <row r="888" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="888" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C888" s="11"/>
     </row>
-    <row r="889" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="889" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C889" s="11"/>
     </row>
-    <row r="890" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="890" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C890" s="11"/>
     </row>
-    <row r="891" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="891" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C891" s="11"/>
     </row>
-    <row r="892" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="892" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C892" s="11"/>
     </row>
-    <row r="893" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="893" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C893" s="11"/>
     </row>
-    <row r="894" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="894" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C894" s="11"/>
     </row>
-    <row r="895" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="895" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C895" s="11"/>
     </row>
-    <row r="896" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="896" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C896" s="11"/>
     </row>
-    <row r="897" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="897" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C897" s="11"/>
     </row>
-    <row r="898" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="898" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C898" s="11"/>
     </row>
-    <row r="899" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="899" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C899" s="11"/>
     </row>
-    <row r="900" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="900" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C900" s="11"/>
     </row>
-    <row r="901" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="901" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C901" s="11"/>
     </row>
-    <row r="902" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="902" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C902" s="11"/>
     </row>
-    <row r="903" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="903" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C903" s="11"/>
     </row>
-    <row r="904" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="904" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C904" s="11"/>
     </row>
-    <row r="905" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="905" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C905" s="11"/>
     </row>
-    <row r="906" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="906" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C906" s="11"/>
     </row>
-    <row r="907" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="907" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C907" s="11"/>
     </row>
-    <row r="908" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="908" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C908" s="11"/>
     </row>
-    <row r="909" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="909" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C909" s="11"/>
     </row>
-    <row r="910" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="910" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C910" s="11"/>
     </row>
-    <row r="911" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="911" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C911" s="11"/>
     </row>
-    <row r="912" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="912" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C912" s="11"/>
     </row>
-    <row r="913" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="913" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C913" s="11"/>
     </row>
-    <row r="914" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="914" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C914" s="11"/>
     </row>
-    <row r="915" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="915" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C915" s="11"/>
     </row>
-    <row r="916" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="916" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C916" s="11"/>
     </row>
-    <row r="917" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="917" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C917" s="11"/>
     </row>
-    <row r="918" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="918" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C918" s="11"/>
     </row>
-    <row r="919" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="919" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C919" s="11"/>
     </row>
-    <row r="920" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="920" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C920" s="11"/>
     </row>
-    <row r="921" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="921" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C921" s="11"/>
     </row>
-    <row r="922" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="922" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C922" s="11"/>
     </row>
-    <row r="923" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="923" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C923" s="11"/>
     </row>
-    <row r="924" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="924" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C924" s="11"/>
     </row>
-    <row r="925" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="925" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C925" s="11"/>
     </row>
-    <row r="926" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="926" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C926" s="11"/>
     </row>
-    <row r="927" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="927" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C927" s="11"/>
     </row>
-    <row r="928" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="928" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C928" s="11"/>
     </row>
-    <row r="929" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="929" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C929" s="11"/>
     </row>
-    <row r="930" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="930" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C930" s="11"/>
     </row>
-    <row r="931" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="931" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C931" s="11"/>
     </row>
-    <row r="932" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="932" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C932" s="11"/>
     </row>
-    <row r="933" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="933" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C933" s="11"/>
     </row>
-    <row r="934" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="934" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C934" s="11"/>
     </row>
-    <row r="935" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="935" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C935" s="11"/>
     </row>
-    <row r="936" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="936" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C936" s="11"/>
     </row>
-    <row r="937" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="937" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C937" s="11"/>
     </row>
-    <row r="938" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="938" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C938" s="11"/>
     </row>
-    <row r="939" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="939" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C939" s="11"/>
     </row>
-    <row r="940" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="940" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C940" s="11"/>
     </row>
-    <row r="941" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="941" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C941" s="11"/>
     </row>
-    <row r="942" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="942" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C942" s="11"/>
     </row>
-    <row r="943" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="943" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C943" s="11"/>
     </row>
-    <row r="944" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="944" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C944" s="11"/>
     </row>
-    <row r="945" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="945" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C945" s="11"/>
     </row>
-    <row r="946" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="946" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C946" s="11"/>
     </row>
-    <row r="947" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="947" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C947" s="11"/>
     </row>
-    <row r="948" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="948" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C948" s="11"/>
     </row>
-    <row r="949" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="949" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C949" s="11"/>
     </row>
-    <row r="950" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="950" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C950" s="11"/>
     </row>
-    <row r="951" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="951" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C951" s="11"/>
     </row>
-    <row r="952" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="952" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C952" s="11"/>
     </row>
-    <row r="953" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="953" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C953" s="11"/>
     </row>
-    <row r="954" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="954" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C954" s="11"/>
     </row>
-    <row r="955" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="955" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C955" s="11"/>
     </row>
-    <row r="956" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="956" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C956" s="11"/>
     </row>
-    <row r="957" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="957" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C957" s="11"/>
     </row>
-    <row r="958" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="958" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C958" s="11"/>
     </row>
-    <row r="959" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="959" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C959" s="11"/>
     </row>
-    <row r="960" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="960" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C960" s="11"/>
     </row>
-    <row r="961" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="961" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C961" s="11"/>
     </row>
-    <row r="962" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="962" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C962" s="11"/>
     </row>
-    <row r="963" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="963" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C963" s="11"/>
     </row>
-    <row r="964" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="964" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C964" s="11"/>
     </row>
-    <row r="965" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="965" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C965" s="11"/>
     </row>
-    <row r="966" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="966" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C966" s="11"/>
     </row>
-    <row r="967" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="967" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C967" s="11"/>
     </row>
-    <row r="968" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="968" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C968" s="11"/>
     </row>
-    <row r="969" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="969" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C969" s="11"/>
     </row>
-    <row r="970" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="970" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C970" s="11"/>
     </row>
-    <row r="971" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="971" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C971" s="11"/>
     </row>
-    <row r="972" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="972" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C972" s="11"/>
     </row>
-    <row r="973" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="973" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C973" s="11"/>
     </row>
-    <row r="974" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="974" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C974" s="11"/>
     </row>
-    <row r="975" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="975" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C975" s="11"/>
     </row>
-    <row r="976" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="976" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C976" s="11"/>
     </row>
-    <row r="977" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="977" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C977" s="11"/>
     </row>
-    <row r="978" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="978" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C978" s="11"/>
     </row>
-    <row r="979" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="979" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C979" s="11"/>
     </row>
-    <row r="980" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="980" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C980" s="11"/>
     </row>
-    <row r="981" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="981" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C981" s="11"/>
     </row>
-    <row r="982" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="982" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C982" s="11"/>
     </row>
-    <row r="983" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="983" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C983" s="11"/>
     </row>
-    <row r="984" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="984" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C984" s="11"/>
     </row>
-    <row r="985" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="985" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C985" s="11"/>
     </row>
-    <row r="986" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="986" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C986" s="11"/>
     </row>
-    <row r="987" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="987" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C987" s="11"/>
     </row>
-    <row r="988" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="988" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C988" s="11"/>
     </row>
-    <row r="989" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="989" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C989" s="11"/>
     </row>
-    <row r="990" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="990" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C990" s="11"/>
     </row>
-    <row r="991" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="991" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C991" s="11"/>
     </row>
-    <row r="992" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="992" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C992" s="11"/>
     </row>
-    <row r="993" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="993" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C993" s="11"/>
     </row>
-    <row r="994" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="994" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C994" s="11"/>
     </row>
-    <row r="995" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="995" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C995" s="11"/>
     </row>
-    <row r="996" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="996" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C996" s="11"/>
     </row>
-    <row r="997" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="997" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C997" s="11"/>
     </row>
-    <row r="998" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="998" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C998" s="11"/>
     </row>
-    <row r="999" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="999" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C999" s="11"/>
     </row>
-    <row r="1000" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1000" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1000" s="11"/>
     </row>
-    <row r="1001" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1001" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1001" s="11"/>
     </row>
-    <row r="1002" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1002" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1002" s="11"/>
     </row>
-    <row r="1003" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1003" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1003" s="11"/>
     </row>
-    <row r="1004" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1004" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1004" s="11"/>
     </row>
-    <row r="1005" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1005" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1005" s="11"/>
     </row>
-    <row r="1006" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1006" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1006" s="11"/>
     </row>
-    <row r="1007" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1007" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1007" s="11"/>
     </row>
-    <row r="1008" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1008" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1008" s="11"/>
     </row>
-    <row r="1009" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1009" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1009" s="11"/>
     </row>
-    <row r="1010" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1010" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1010" s="11"/>
     </row>
-    <row r="1011" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1011" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1011" s="11"/>
     </row>
-    <row r="1012" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1012" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1012" s="11"/>
     </row>
-    <row r="1013" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1013" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1013" s="11"/>
     </row>
-    <row r="1014" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1014" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1014" s="11"/>
     </row>
-    <row r="1015" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1015" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1015" s="11"/>
     </row>
-    <row r="1016" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1016" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1016" s="11"/>
     </row>
-    <row r="1017" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1017" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1017" s="11"/>
     </row>
-    <row r="1018" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1018" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1018" s="11"/>
     </row>
-    <row r="1019" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1020" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1021" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1022" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1023" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1024" spans="3:3" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1025" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1026" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1027" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1028" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="1019" spans="3:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1020" spans="3:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1021" spans="3:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1022" spans="3:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1023" spans="3:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1024" spans="3:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1025" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1026" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1027" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="1028" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:F2"/>
@@ -4071,10 +4113,11 @@
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D27:F27"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C23 C24:C1018" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C1018" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No,Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>